<commit_message>
Añade saldos iniciniciales y finales esperados a el ejemplo de la caratula de proveedores
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -113,10 +113,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -149,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,8 +205,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -279,42 +286,141 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -322,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -330,17 +436,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,18 +464,41 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -386,6 +506,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -687,73 +812,85 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
+      <c r="B3" s="42">
+        <v>8867057.4600000009</v>
+      </c>
+      <c r="C3" s="43">
+        <v>27863597.690000001</v>
+      </c>
+      <c r="D3" s="43">
+        <v>164664345</v>
+      </c>
+      <c r="E3" s="43">
+        <v>27863597.690000001</v>
+      </c>
+      <c r="F3" s="22">
+        <f>D3+E3</f>
+        <v>192527942.69</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -774,12 +911,12 @@
       <c r="F4" s="4">
         <v>-2.2662000000000004</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>2.46</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="5">
-        <f>F4-G4</f>
+        <f t="shared" ref="I4:I10" si="0">F4-G4</f>
         <v>-4.7262000000000004</v>
       </c>
     </row>
@@ -802,12 +939,12 @@
       <c r="F5" s="4">
         <v>-30076216.312899999</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <v>-30076216.319999993</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="6">
-        <f>F5-G5</f>
+        <f t="shared" si="0"/>
         <v>7.0999935269355774E-3</v>
       </c>
     </row>
@@ -830,12 +967,12 @@
       <c r="F6" s="4">
         <v>-206275.19480000148</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>-189332.92999999996</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6">
-        <f>F6-G6</f>
+        <f t="shared" si="0"/>
         <v>-16942.264800001518</v>
       </c>
     </row>
@@ -854,12 +991,12 @@
       <c r="F7" s="4">
         <v>146948.69279999999</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <v>146948.69</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="6">
-        <f>F7-G7</f>
+        <f t="shared" si="0"/>
         <v>2.7999999874737114E-3</v>
       </c>
     </row>
@@ -878,12 +1015,12 @@
       <c r="F8" s="4">
         <v>0</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <v>0</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <f>F8-G8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -906,15 +1043,15 @@
       <c r="F9" s="4">
         <v>-854708.85509999993</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <v>-715496.49</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="5">
-        <f>F9-G9</f>
+        <f t="shared" si="0"/>
         <v>-139212.36509999994</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -931,12 +1068,12 @@
       <c r="F10" s="4">
         <v>-44064.056199999999</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="16">
         <v>-44064.06</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="6">
-        <f>F10-G10</f>
+        <f t="shared" si="0"/>
         <v>3.7999999985913746E-3</v>
       </c>
     </row>
@@ -959,12 +1096,12 @@
       <c r="F11" s="4">
         <v>-227522.61490000002</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <v>-227522.62000000002</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="6">
-        <f t="shared" ref="I11:I22" si="0">F11-G11</f>
+        <f t="shared" ref="I11:I22" si="1">F11-G11</f>
         <v>5.100000009406358E-3</v>
       </c>
     </row>
@@ -987,12 +1124,12 @@
       <c r="F12" s="4">
         <v>45878999.255799979</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <v>45878999.320000015</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.4200036227703094E-2</v>
       </c>
     </row>
@@ -1011,12 +1148,12 @@
       <c r="F13" s="4">
         <v>91963867.380400062</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <v>91963867.389999986</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.5999240875244141E-3</v>
       </c>
     </row>
@@ -1039,12 +1176,12 @@
       <c r="F14" s="4">
         <v>2421621.6485000001</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="16">
         <v>2421621.649999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.4999988488852978E-3</v>
       </c>
     </row>
@@ -1063,15 +1200,15 @@
       <c r="F15" s="4">
         <v>303015.25</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <v>0</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>303015.25</v>
       </c>
-      <c r="J15" s="17"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1092,12 +1229,12 @@
       <c r="F16" s="4">
         <v>2262817.2611999996</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="16">
         <v>2262817.2499999991</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1200000531971455E-2</v>
       </c>
     </row>
@@ -1120,12 +1257,12 @@
       <c r="F17" s="4">
         <v>580292.97050000005</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="16">
         <v>580292.95000000007</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0499999984167516E-2</v>
       </c>
     </row>
@@ -1144,12 +1281,12 @@
       <c r="F18" s="4">
         <v>2282441.5255999998</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="16">
         <v>2282441.52</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.59999980032444E-3</v>
       </c>
     </row>
@@ -1172,12 +1309,12 @@
       <c r="F19" s="4">
         <v>30241758.399500046</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="16">
         <v>30074302.809999984</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>167455.58950006217</v>
       </c>
     </row>
@@ -1200,12 +1337,12 @@
       <c r="F20" s="4">
         <v>-118813932.70550004</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="16">
         <v>-118656140.56000003</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-157792.14550000429</v>
       </c>
     </row>
@@ -1224,12 +1361,12 @@
       <c r="F21" s="4">
         <v>6961029.4586000061</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="16">
         <v>6961029.4400000004</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8600005656480789E-2</v>
       </c>
     </row>
@@ -1244,65 +1381,107 @@
       <c r="D22" s="4">
         <v>-72995.217700000008</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21">
+      <c r="E22" s="17"/>
+      <c r="F22" s="18">
         <v>-72995.217700000008</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="19">
         <v>-72995.209999999992</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="23">
-        <f t="shared" si="0"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="20">
+        <f t="shared" si="1"/>
         <v>-7.7000000164844096E-3</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="31">
-        <f>SUM(B2:B22)</f>
-        <v>939064.59939999972</v>
-      </c>
-      <c r="C23" s="31">
-        <f>SUM(C2:C22)</f>
-        <v>4947228.247699976</v>
-      </c>
-      <c r="D23" s="31">
-        <f>SUM(D2:D22)</f>
-        <v>27799846.370900061</v>
-      </c>
-      <c r="E23" s="31">
-        <f>SUM(E2:E22)</f>
-        <v>4947228.2486999929</v>
-      </c>
-      <c r="F23" s="31">
-        <f>SUM(F2:F22)</f>
-        <v>32747074.619600054</v>
-      </c>
-      <c r="G23" s="31">
-        <f>SUM(G2:G22)</f>
+      <c r="B23" s="29">
+        <f t="shared" ref="B23:I23" si="2">SUM(B2:B22)</f>
+        <v>9806122.0594000015</v>
+      </c>
+      <c r="C23" s="29">
+        <f t="shared" si="2"/>
+        <v>32810825.937699974</v>
+      </c>
+      <c r="D23" s="29">
+        <f t="shared" si="2"/>
+        <v>192464191.37090006</v>
+      </c>
+      <c r="E23" s="29">
+        <f t="shared" si="2"/>
+        <v>32810825.938699991</v>
+      </c>
+      <c r="F23" s="29">
+        <f t="shared" si="2"/>
+        <v>225275017.30960011</v>
+      </c>
+      <c r="G23" s="29">
+        <f t="shared" si="2"/>
         <v>32590555.289999973</v>
       </c>
-      <c r="H23" s="31">
-        <f>SUM(H2:H22)</f>
+      <c r="H23" s="29">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="31">
-        <f>SUM(I2:I22)</f>
+      <c r="I23" s="29">
+        <f t="shared" si="2"/>
         <v>156519.32960009674</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="B24" s="37">
+        <v>9805347.0899999999</v>
+      </c>
+      <c r="C24" s="37">
+        <v>32806116.399999999</v>
+      </c>
+      <c r="D24" s="37">
+        <v>192473715.09999999</v>
+      </c>
+      <c r="E24" s="37">
+        <v>32806116.399999999</v>
+      </c>
+      <c r="F24" s="38">
+        <f>D24+E24</f>
+        <v>225279831.5</v>
+      </c>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="41"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
         <v>1</v>
       </c>
+      <c r="B25" s="30">
+        <f>B24-B23</f>
+        <v>-774.96940000168979</v>
+      </c>
+      <c r="C25" s="30">
+        <f>C24-C23</f>
+        <v>-4709.5376999750733</v>
+      </c>
+      <c r="D25" s="30">
+        <f t="shared" ref="D25:F25" si="3">D24-D23</f>
+        <v>9523.7290999293327</v>
+      </c>
+      <c r="E25" s="30">
+        <f t="shared" si="3"/>
+        <v>-4709.5386999920011</v>
+      </c>
+      <c r="F25" s="30">
+        <f t="shared" si="3"/>
+        <v>4814.1903998851776</v>
+      </c>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Añade observaciones al ejemplo de la caratula de proveedores
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18960" windowHeight="7995" tabRatio="427"/>
   </bookViews>
   <sheets>
     <sheet name="SEP" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>concepto</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>Saldo Inicial Antigüedad</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Son los que se habian detecado con anterioridad. Los que vienen directos de cxp</t>
+  </si>
+  <si>
+    <t>No tiene configuada la Poliza Contable</t>
+  </si>
+  <si>
+    <t>La diferencia ya esta validada y tiene una diferencia de como 1000 contra lo que habian identificado en Contabilidad</t>
+  </si>
+  <si>
+    <t>Estos saldos Iniciales, fueron obtenidos del reporte de Antigüedad que esta en la intranet</t>
+  </si>
+  <si>
+    <t>Hay que revisar el reporte de la intranet, al parecer no esta considerando algunas transacciones que es  lo que provoca esta diferencia</t>
   </si>
 </sst>
 </file>
@@ -117,7 +135,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
-    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -150,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +229,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -260,19 +296,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -364,7 +387,85 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -382,34 +483,19 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -428,77 +514,174 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -812,680 +995,719 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="42" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
-    </row>
-    <row r="2" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="J2" s="47"/>
+    </row>
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="38">
         <v>8867057.4600000009</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="15">
         <v>27863597.690000001</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="15">
         <v>164664345</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="15">
         <v>27863597.690000001</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="14">
         <f>D3+E3</f>
         <v>192527942.69</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="50" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="39">
         <v>-0.11949999999999997</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="19">
         <v>-1.32E-2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="19">
         <v>-2.2530000000000006</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="19">
         <v>-1.32E-2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="19">
         <v>-2.2662000000000004</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="20">
         <v>2.46</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="5">
+      <c r="H4" s="21"/>
+      <c r="I4" s="22">
         <f t="shared" ref="I4:I10" si="0">F4-G4</f>
         <v>-4.7262000000000004</v>
       </c>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="39">
         <v>-1595235.69</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="19">
         <v>-119347.66</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="19">
         <v>-29956868.653000001</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="19">
         <v>-119347.6599</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="19">
         <v>-30076216.312899999</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="20">
         <v>-30076216.319999993</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6">
+      <c r="H5" s="21"/>
+      <c r="I5" s="23">
         <f t="shared" si="0"/>
         <v>7.0999935269355774E-3</v>
       </c>
+      <c r="J5" s="48"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="39">
         <v>-2.4199999978009146E-2</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="19">
         <v>1.999999993131496E-3</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="19">
         <v>-206275.19670000148</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="19">
         <v>1.9000000029336661E-3</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="19">
         <v>-206275.19480000148</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="20">
         <v>-189332.92999999996</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6">
+      <c r="H6" s="21"/>
+      <c r="I6" s="23">
         <f t="shared" si="0"/>
         <v>-16942.264800001518</v>
       </c>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="39">
         <v>7534.1304000000009</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19">
         <v>146948.69279999999</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="4">
+      <c r="E7" s="21"/>
+      <c r="F7" s="19">
         <v>146948.69279999999</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="20">
         <v>146948.69</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6">
+      <c r="H7" s="21"/>
+      <c r="I7" s="23">
         <f t="shared" si="0"/>
         <v>2.7999999874737114E-3</v>
       </c>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="39">
         <v>0</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19">
         <v>0</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="4">
+      <c r="E8" s="21"/>
+      <c r="F8" s="19">
         <v>0</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="20">
         <v>0</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="H8" s="21"/>
+      <c r="I8" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="39">
         <v>-43798.515700000004</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="19">
         <v>-3502</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="19">
         <v>-851206.85509999993</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="19">
         <v>-3502</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="19">
         <v>-854708.85509999993</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="20">
         <v>-715496.49</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="5">
+      <c r="H9" s="21"/>
+      <c r="I9" s="22">
         <f t="shared" si="0"/>
         <v>-139212.36509999994</v>
       </c>
-      <c r="J9" s="14"/>
+      <c r="J9" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="39">
         <v>-2336.2399999999998</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19">
         <v>-44064.056199999999</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="4">
+      <c r="E10" s="21"/>
+      <c r="F10" s="19">
         <v>-44064.056199999999</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="20">
         <v>-44064.06</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="6">
+      <c r="H10" s="21"/>
+      <c r="I10" s="23">
         <f t="shared" si="0"/>
         <v>3.7999999985913746E-3</v>
       </c>
+      <c r="J10" s="48"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="39">
         <v>-10301.460000000001</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="19">
         <v>-23222</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="19">
         <v>-204300.61490000002</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="19">
         <v>-23222</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="19">
         <v>-227522.61490000002</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="20">
         <v>-227522.62000000002</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="6">
+      <c r="H11" s="21"/>
+      <c r="I11" s="23">
         <f t="shared" ref="I11:I22" si="1">F11-G11</f>
         <v>5.100000009406358E-3</v>
       </c>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="39">
         <v>2273843.7274000007</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="19">
         <v>2093582.8945000002</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="19">
         <v>43785416.364299983</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="19">
         <v>2093582.8914999997</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="19">
         <v>45878999.255799979</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="20">
         <v>45878999.320000015</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="6">
+      <c r="H12" s="21"/>
+      <c r="I12" s="23">
         <f t="shared" si="1"/>
         <v>-6.4200036227703094E-2</v>
       </c>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="39">
         <v>4812894.9151000027</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19">
         <v>91963867.380400062</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4">
+      <c r="E13" s="21"/>
+      <c r="F13" s="19">
         <v>91963867.380400062</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="20">
         <v>91963867.389999986</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="6">
+      <c r="H13" s="21"/>
+      <c r="I13" s="23">
         <f t="shared" si="1"/>
         <v>-9.5999240875244141E-3</v>
       </c>
+      <c r="J13" s="48"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="39">
         <v>76408.107199999999</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="19">
         <v>953091.40320000006</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="19">
         <v>1468530.2485000005</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="19">
         <v>953091.39999999979</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="19">
         <v>2421621.6485000001</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="20">
         <v>2421621.649999999</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="6">
+      <c r="H14" s="21"/>
+      <c r="I14" s="23">
         <f t="shared" si="1"/>
         <v>-1.4999988488852978E-3</v>
       </c>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="39">
         <v>15693.570400000001</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19">
         <v>303015.25</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="4">
+      <c r="E15" s="21"/>
+      <c r="F15" s="19">
         <v>303015.25</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="20">
         <v>0</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="6">
+      <c r="H15" s="21"/>
+      <c r="I15" s="23">
         <f t="shared" si="1"/>
         <v>303015.25</v>
       </c>
-      <c r="J15" s="14"/>
+      <c r="J15" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="39">
         <v>6543.9660000000003</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="19">
         <v>2140154.8114</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="19">
         <v>122662.45500000002</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="19">
         <v>2140154.8061999995</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="19">
         <v>2262817.2611999996</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="20">
         <v>2262817.2499999991</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="6">
+      <c r="H16" s="21"/>
+      <c r="I16" s="23">
         <f t="shared" si="1"/>
         <v>1.1200000531971455E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="J16" s="48"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="39">
         <v>6003.77</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="19">
         <v>467240.33000000007</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="19">
         <v>113052.64079999999</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="19">
         <v>467240.32970000006</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="19">
         <v>580292.97050000005</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="20">
         <v>580292.95000000007</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="6">
+      <c r="H17" s="21"/>
+      <c r="I17" s="23">
         <f t="shared" si="1"/>
         <v>2.0499999984167516E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="J17" s="48"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4">
+      <c r="B18" s="39"/>
+      <c r="C18" s="19">
         <v>2282441.5276000001</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="4">
+      <c r="D18" s="21"/>
+      <c r="E18" s="19">
         <v>2282441.5255999998</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="19">
         <v>2282441.5255999998</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="20">
         <v>2282441.52</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="6">
+      <c r="H18" s="21"/>
+      <c r="I18" s="23">
         <f t="shared" si="1"/>
         <v>5.59999980032444E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="J18" s="48"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="39">
         <v>91197.16</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="19">
         <v>28497266.538799923</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="19">
         <v>1744491.8740000001</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="19">
         <v>28497266.525500044</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="19">
         <v>30241758.399500046</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="20">
         <v>30074302.809999984</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="6">
+      <c r="H19" s="21"/>
+      <c r="I19" s="23">
         <f t="shared" si="1"/>
         <v>167455.58950006217</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="J19" s="48"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="39">
         <v>-4699382.6977000032</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="19">
         <v>-31340477.586599946</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="19">
         <v>-87473455.146899983</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="19">
         <v>-31340477.558600053</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="19">
         <v>-118813932.70550004</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="20">
         <v>-118656140.56000003</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="6">
+      <c r="H20" s="21"/>
+      <c r="I20" s="23">
         <f t="shared" si="1"/>
         <v>-157792.14550000429</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="J20" s="48"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="39">
         <v>0</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
+      <c r="C21" s="19"/>
+      <c r="D21" s="19">
         <v>6961029.4586000061</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="4">
+      <c r="E21" s="21"/>
+      <c r="F21" s="19">
         <v>6961029.4586000061</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="20">
         <v>6961029.4400000004</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="6">
+      <c r="H21" s="21"/>
+      <c r="I21" s="23">
         <f t="shared" si="1"/>
         <v>1.8600005656480789E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="J21" s="48"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="39">
         <v>0</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4">
+      <c r="C22" s="19"/>
+      <c r="D22" s="19">
         <v>-72995.217700000008</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18">
+      <c r="E22" s="25"/>
+      <c r="F22" s="26">
         <v>-72995.217700000008</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="27">
         <v>-72995.209999999992</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="20">
+      <c r="H22" s="25"/>
+      <c r="I22" s="28">
         <f t="shared" si="1"/>
         <v>-7.7000000164844096E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="J22" s="48"/>
+    </row>
+    <row r="23" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="40">
         <f t="shared" ref="B23:I23" si="2">SUM(B2:B22)</f>
         <v>9806122.0594000015</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="30">
         <f t="shared" si="2"/>
         <v>32810825.937699974</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="30">
         <f t="shared" si="2"/>
         <v>192464191.37090006</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="30">
         <f t="shared" si="2"/>
         <v>32810825.938699991</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>225275017.30960011</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="30">
         <f t="shared" si="2"/>
         <v>32590555.289999973</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="29">
+      <c r="I23" s="56">
         <f t="shared" si="2"/>
         <v>156519.32960009674</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="J23" s="45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="37">
+      <c r="B24" s="41">
         <v>9805347.0899999999</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="32">
         <v>32806116.399999999</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="32">
         <v>192473715.09999999</v>
       </c>
-      <c r="E24" s="37">
+      <c r="E24" s="32">
         <v>32806116.399999999</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="33">
         <f>D24+E24</f>
         <v>225279831.5</v>
       </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="37">
         <f>B24-B23</f>
         <v>-774.96940000168979</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="37">
         <f>C24-C23</f>
         <v>-4709.5376999750733</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="37">
         <f t="shared" ref="D25:F25" si="3">D24-D23</f>
         <v>9523.7290999293327</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="37">
         <f t="shared" si="3"/>
         <v>-4709.5386999920011</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="37">
         <f t="shared" si="3"/>
         <v>4814.1903998851776</v>
       </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="33"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="55" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualiza observaciones eejemplo caratula de proveedores
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -118,13 +118,13 @@
     <t>No tiene configuada la Poliza Contable</t>
   </si>
   <si>
-    <t>La diferencia ya esta validada y tiene una diferencia de como 1000 contra lo que habian identificado en Contabilidad</t>
-  </si>
-  <si>
     <t>Estos saldos Iniciales, fueron obtenidos del reporte de Antigüedad que esta en la intranet</t>
   </si>
   <si>
-    <t>Hay que revisar el reporte de la intranet, al parecer no esta considerando algunas transacciones que es  lo que provoca esta diferencia</t>
+    <t>La diferencia cuadra con la que se habia identificado previamente.</t>
+  </si>
+  <si>
+    <t>Hay que revisar el reporte de la intranet, al parecer no esta considerando algunas transacciones lo que provoca esta diferencia</t>
   </si>
 </sst>
 </file>
@@ -535,152 +535,152 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -992,47 +992,47 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="42" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73" style="49" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="46" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1054,196 +1054,196 @@
       <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="47"/>
+      <c r="J2" s="56"/>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="36">
         <v>8867057.4600000009</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>27863597.690000001</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <v>164664345</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="13">
         <v>27863597.690000001</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <f>D3+E3</f>
         <v>192527942.69</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="50" t="s">
-        <v>35</v>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="46" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="37">
         <v>-0.11949999999999997</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="17">
         <v>-1.32E-2</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="17">
         <v>-2.2530000000000006</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>-1.32E-2</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="17">
         <v>-2.2662000000000004</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="18">
         <v>2.46</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22">
+      <c r="H4" s="19"/>
+      <c r="I4" s="20">
         <f t="shared" ref="I4:I10" si="0">F4-G4</f>
         <v>-4.7262000000000004</v>
       </c>
-      <c r="J4" s="48"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>-1595235.69</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <v>-119347.66</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="17">
         <v>-29956868.653000001</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>-119347.6599</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="17">
         <v>-30076216.312899999</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>-30076216.319999993</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="23">
+      <c r="H5" s="19"/>
+      <c r="I5" s="21">
         <f t="shared" si="0"/>
         <v>7.0999935269355774E-3</v>
       </c>
-      <c r="J5" s="48"/>
+      <c r="J5" s="44"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>-2.4199999978009146E-2</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="17">
         <v>1.999999993131496E-3</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <v>-206275.19670000148</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>1.9000000029336661E-3</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <v>-206275.19480000148</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="18">
         <v>-189332.92999999996</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="23">
+      <c r="H6" s="19"/>
+      <c r="I6" s="21">
         <f t="shared" si="0"/>
         <v>-16942.264800001518</v>
       </c>
-      <c r="J6" s="48"/>
+      <c r="J6" s="44"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>7534.1304000000009</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17">
         <v>146948.69279999999</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="19">
+      <c r="E7" s="19"/>
+      <c r="F7" s="17">
         <v>146948.69279999999</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="18">
         <v>146948.69</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="23">
+      <c r="H7" s="19"/>
+      <c r="I7" s="21">
         <f t="shared" si="0"/>
         <v>2.7999999874737114E-3</v>
       </c>
-      <c r="J7" s="48"/>
+      <c r="J7" s="44"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>0</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17">
         <v>0</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="19">
+      <c r="E8" s="19"/>
+      <c r="F8" s="17">
         <v>0</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="18">
         <v>0</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="24">
+      <c r="H8" s="19"/>
+      <c r="I8" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="48"/>
+      <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>-43798.515700000004</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="17">
         <v>-3502</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <v>-851206.85509999993</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>-3502</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <v>-854708.85509999993</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="18">
         <v>-715496.49</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22">
+      <c r="H9" s="19"/>
+      <c r="I9" s="20">
         <f t="shared" si="0"/>
         <v>-139212.36509999994</v>
       </c>
@@ -1252,162 +1252,162 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>-2336.2399999999998</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17">
         <v>-44064.056199999999</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="19">
+      <c r="E10" s="19"/>
+      <c r="F10" s="17">
         <v>-44064.056199999999</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="18">
         <v>-44064.06</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="23">
+      <c r="H10" s="19"/>
+      <c r="I10" s="21">
         <f t="shared" si="0"/>
         <v>3.7999999985913746E-3</v>
       </c>
-      <c r="J10" s="48"/>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>-10301.460000000001</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <v>-23222</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="17">
         <v>-204300.61490000002</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="17">
         <v>-23222</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="17">
         <v>-227522.61490000002</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="18">
         <v>-227522.62000000002</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="23">
+      <c r="H11" s="19"/>
+      <c r="I11" s="21">
         <f t="shared" ref="I11:I22" si="1">F11-G11</f>
         <v>5.100000009406358E-3</v>
       </c>
-      <c r="J11" s="48"/>
+      <c r="J11" s="44"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>2273843.7274000007</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="17">
         <v>2093582.8945000002</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="17">
         <v>43785416.364299983</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="17">
         <v>2093582.8914999997</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="17">
         <v>45878999.255799979</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="18">
         <v>45878999.320000015</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="23">
+      <c r="H12" s="19"/>
+      <c r="I12" s="21">
         <f t="shared" si="1"/>
         <v>-6.4200036227703094E-2</v>
       </c>
-      <c r="J12" s="48"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>4812894.9151000027</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17">
         <v>91963867.380400062</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="19">
+      <c r="E13" s="19"/>
+      <c r="F13" s="17">
         <v>91963867.380400062</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="18">
         <v>91963867.389999986</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="23">
+      <c r="H13" s="19"/>
+      <c r="I13" s="21">
         <f t="shared" si="1"/>
         <v>-9.5999240875244141E-3</v>
       </c>
-      <c r="J13" s="48"/>
+      <c r="J13" s="44"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="37">
         <v>76408.107199999999</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="17">
         <v>953091.40320000006</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="17">
         <v>1468530.2485000005</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="17">
         <v>953091.39999999979</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="17">
         <v>2421621.6485000001</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="18">
         <v>2421621.649999999</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="23">
+      <c r="H14" s="19"/>
+      <c r="I14" s="21">
         <f t="shared" si="1"/>
         <v>-1.4999988488852978E-3</v>
       </c>
-      <c r="J14" s="48"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="37">
         <v>15693.570400000001</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17">
         <v>303015.25</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19">
+      <c r="E15" s="19"/>
+      <c r="F15" s="17">
         <v>303015.25</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="18">
         <v>0</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="23">
+      <c r="H15" s="19"/>
+      <c r="I15" s="21">
         <f t="shared" si="1"/>
         <v>303015.25</v>
       </c>
@@ -1416,291 +1416,291 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B16" s="37">
         <v>6543.9660000000003</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="17">
         <v>2140154.8114</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="17">
         <v>122662.45500000002</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="17">
         <v>2140154.8061999995</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="17">
         <v>2262817.2611999996</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="18">
         <v>2262817.2499999991</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="23">
+      <c r="H16" s="19"/>
+      <c r="I16" s="21">
         <f t="shared" si="1"/>
         <v>1.1200000531971455E-2</v>
       </c>
-      <c r="J16" s="48"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="39">
+      <c r="B17" s="37">
         <v>6003.77</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <v>467240.33000000007</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="17">
         <v>113052.64079999999</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="17">
         <v>467240.32970000006</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="17">
         <v>580292.97050000005</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="18">
         <v>580292.95000000007</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="23">
+      <c r="H17" s="19"/>
+      <c r="I17" s="21">
         <f t="shared" si="1"/>
         <v>2.0499999984167516E-2</v>
       </c>
-      <c r="J17" s="48"/>
+      <c r="J17" s="44"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="19">
+      <c r="B18" s="37"/>
+      <c r="C18" s="17">
         <v>2282441.5276000001</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="19">
+      <c r="D18" s="19"/>
+      <c r="E18" s="17">
         <v>2282441.5255999998</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="17">
         <v>2282441.5255999998</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="18">
         <v>2282441.52</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="23">
+      <c r="H18" s="19"/>
+      <c r="I18" s="21">
         <f t="shared" si="1"/>
         <v>5.59999980032444E-3</v>
       </c>
-      <c r="J18" s="48"/>
+      <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="39">
+      <c r="B19" s="37">
         <v>91197.16</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="17">
         <v>28497266.538799923</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="17">
         <v>1744491.8740000001</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <v>28497266.525500044</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="17">
         <v>30241758.399500046</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="18">
         <v>30074302.809999984</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="23">
+      <c r="H19" s="19"/>
+      <c r="I19" s="21">
         <f t="shared" si="1"/>
         <v>167455.58950006217</v>
       </c>
-      <c r="J19" s="48"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="39">
+      <c r="B20" s="37">
         <v>-4699382.6977000032</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="17">
         <v>-31340477.586599946</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="17">
         <v>-87473455.146899983</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="17">
         <v>-31340477.558600053</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="17">
         <v>-118813932.70550004</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="18">
         <v>-118656140.56000003</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="23">
+      <c r="H20" s="19"/>
+      <c r="I20" s="21">
         <f t="shared" si="1"/>
         <v>-157792.14550000429</v>
       </c>
-      <c r="J20" s="48"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="39">
+      <c r="B21" s="37">
         <v>0</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <v>6961029.4586000061</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="19">
+      <c r="E21" s="19"/>
+      <c r="F21" s="17">
         <v>6961029.4586000061</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="18">
         <v>6961029.4400000004</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="23">
+      <c r="H21" s="19"/>
+      <c r="I21" s="21">
         <f t="shared" si="1"/>
         <v>1.8600005656480789E-2</v>
       </c>
-      <c r="J21" s="48"/>
+      <c r="J21" s="44"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="39">
+      <c r="B22" s="37">
         <v>0</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <v>-72995.217700000008</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26">
+      <c r="E22" s="23"/>
+      <c r="F22" s="24">
         <v>-72995.217700000008</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="25">
         <v>-72995.209999999992</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="28">
+      <c r="H22" s="23"/>
+      <c r="I22" s="26">
         <f t="shared" si="1"/>
         <v>-7.7000000164844096E-3</v>
       </c>
-      <c r="J22" s="48"/>
-    </row>
-    <row r="23" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="J22" s="44"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="38">
         <f t="shared" ref="B23:I23" si="2">SUM(B2:B22)</f>
         <v>9806122.0594000015</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="28">
         <f t="shared" si="2"/>
         <v>32810825.937699974</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="28">
         <f t="shared" si="2"/>
         <v>192464191.37090006</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="28">
         <f t="shared" si="2"/>
         <v>32810825.938699991</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="28">
         <f t="shared" si="2"/>
         <v>225275017.30960011</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="28">
         <f t="shared" si="2"/>
         <v>32590555.289999973</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="56">
+      <c r="I23" s="52">
         <f t="shared" si="2"/>
         <v>156519.32960009674</v>
       </c>
-      <c r="J23" s="45" t="s">
-        <v>34</v>
+      <c r="J23" s="43" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="41">
+      <c r="B24" s="39">
         <v>9805347.0899999999</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="30">
         <v>32806116.399999999</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="30">
         <v>192473715.09999999</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="30">
         <v>32806116.399999999</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="31">
         <f>D24+E24</f>
         <v>225279831.5</v>
       </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="50" t="s">
-        <v>35</v>
+      <c r="G24" s="32"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="46" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="37">
+      <c r="B25" s="35">
         <f>B24-B23</f>
         <v>-774.96940000168979</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="35">
         <f>C24-C23</f>
         <v>-4709.5376999750733</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="35">
         <f t="shared" ref="D25:F25" si="3">D24-D23</f>
         <v>9523.7290999293327</v>
       </c>
-      <c r="E25" s="37">
+      <c r="E25" s="35">
         <f t="shared" si="3"/>
         <v>-4709.5386999920011</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="35">
         <f t="shared" si="3"/>
         <v>4814.1903998851776</v>
       </c>
-      <c r="G25" s="52"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="55" t="s">
+      <c r="G25" s="48"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="51" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualiza Cabeceros ejemplo caratula cxp
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>concepto</t>
   </si>
@@ -22,24 +22,9 @@
     <t>Variacion</t>
   </si>
   <si>
-    <t>modulo cxc dlls conversion</t>
-  </si>
-  <si>
-    <t>modulo cxc mn</t>
-  </si>
-  <si>
-    <t>total modulo cxc</t>
-  </si>
-  <si>
     <t>CONCILIACION MODULO CXP VS MODULO CONTABILIDAD</t>
   </si>
   <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>Dolares</t>
-  </si>
-  <si>
     <t>Reevaluacion Credito</t>
   </si>
   <si>
@@ -125,6 +110,18 @@
   </si>
   <si>
     <t>Hay que revisar el reporte de la intranet, al parecer no esta considerando algunas transacciones lo que provoca esta diferencia</t>
+  </si>
+  <si>
+    <t>Cartera Dolares</t>
+  </si>
+  <si>
+    <t>Cartera MXN</t>
+  </si>
+  <si>
+    <t>Cartera Dlls Conversion</t>
+  </si>
+  <si>
+    <t>Total Cartera</t>
   </si>
 </sst>
 </file>
@@ -514,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -522,9 +519,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -538,9 +532,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -556,9 +547,6 @@
     <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,9 +596,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,9 +643,6 @@
     <xf numFmtId="43" fontId="0" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -681,6 +663,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,725 +974,696 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="40" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73" style="45" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="55" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>7</v>
+      <c r="B2" s="52" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="56"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="36">
+      <c r="I2" s="51"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="32">
         <v>8867057.4600000009</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>27863597.690000001</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="11">
         <v>164664345</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>27863597.690000001</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <f>D3+E3</f>
         <v>192527942.69</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="33">
+        <v>-0.11949999999999997</v>
+      </c>
+      <c r="C4" s="14">
+        <v>-1.32E-2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-2.2530000000000006</v>
+      </c>
+      <c r="E4" s="14">
+        <v>-1.32E-2</v>
+      </c>
+      <c r="F4" s="14">
+        <v>-2.2662000000000004</v>
+      </c>
+      <c r="G4" s="15">
+        <v>2.46</v>
+      </c>
+      <c r="H4" s="17">
+        <f>F4-G4</f>
+        <v>-4.7262000000000004</v>
+      </c>
+      <c r="I4" s="40"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="33">
+        <v>-1595235.69</v>
+      </c>
+      <c r="C5" s="14">
+        <v>-119347.66</v>
+      </c>
+      <c r="D5" s="14">
+        <v>-29956868.653000001</v>
+      </c>
+      <c r="E5" s="14">
+        <v>-119347.6599</v>
+      </c>
+      <c r="F5" s="14">
+        <v>-30076216.312899999</v>
+      </c>
+      <c r="G5" s="15">
+        <v>-30076216.319999993</v>
+      </c>
+      <c r="H5" s="18">
+        <f>F5-G5</f>
+        <v>7.0999935269355774E-3</v>
+      </c>
+      <c r="I5" s="40"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="33">
+        <v>-2.4199999978009146E-2</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1.999999993131496E-3</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-206275.19670000148</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1.9000000029336661E-3</v>
+      </c>
+      <c r="F6" s="14">
+        <v>-206275.19480000148</v>
+      </c>
+      <c r="G6" s="15">
+        <v>-189332.92999999996</v>
+      </c>
+      <c r="H6" s="18">
+        <f>F6-G6</f>
+        <v>-16942.264800001518</v>
+      </c>
+      <c r="I6" s="40"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="33">
+        <v>7534.1304000000009</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14">
+        <v>146948.69279999999</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="14">
+        <v>146948.69279999999</v>
+      </c>
+      <c r="G7" s="15">
+        <v>146948.69</v>
+      </c>
+      <c r="H7" s="18">
+        <f>F7-G7</f>
+        <v>2.7999999874737114E-3</v>
+      </c>
+      <c r="I7" s="40"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="19">
+        <f>F8-G8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="37">
-        <v>-0.11949999999999997</v>
-      </c>
-      <c r="C4" s="17">
-        <v>-1.32E-2</v>
-      </c>
-      <c r="D4" s="17">
-        <v>-2.2530000000000006</v>
-      </c>
-      <c r="E4" s="17">
-        <v>-1.32E-2</v>
-      </c>
-      <c r="F4" s="17">
-        <v>-2.2662000000000004</v>
-      </c>
-      <c r="G4" s="18">
-        <v>2.46</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20">
-        <f t="shared" ref="I4:I10" si="0">F4-G4</f>
-        <v>-4.7262000000000004</v>
-      </c>
-      <c r="J4" s="44"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="B9" s="33">
+        <v>-43798.515700000004</v>
+      </c>
+      <c r="C9" s="14">
+        <v>-3502</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-851206.85509999993</v>
+      </c>
+      <c r="E9" s="14">
+        <v>-3502</v>
+      </c>
+      <c r="F9" s="14">
+        <v>-854708.85509999993</v>
+      </c>
+      <c r="G9" s="15">
+        <v>-715496.49</v>
+      </c>
+      <c r="H9" s="17">
+        <f>F9-G9</f>
+        <v>-139212.36509999994</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="37">
-        <v>-1595235.69</v>
-      </c>
-      <c r="C5" s="17">
-        <v>-119347.66</v>
-      </c>
-      <c r="D5" s="17">
-        <v>-29956868.653000001</v>
-      </c>
-      <c r="E5" s="17">
-        <v>-119347.6599</v>
-      </c>
-      <c r="F5" s="17">
-        <v>-30076216.312899999</v>
-      </c>
-      <c r="G5" s="18">
-        <v>-30076216.319999993</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="21">
+      <c r="B10" s="33">
+        <v>-2336.2399999999998</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14">
+        <v>-44064.056199999999</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="14">
+        <v>-44064.056199999999</v>
+      </c>
+      <c r="G10" s="15">
+        <v>-44064.06</v>
+      </c>
+      <c r="H10" s="18">
+        <f>F10-G10</f>
+        <v>3.7999999985913746E-3</v>
+      </c>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="33">
+        <v>-10301.460000000001</v>
+      </c>
+      <c r="C11" s="14">
+        <v>-23222</v>
+      </c>
+      <c r="D11" s="14">
+        <v>-204300.61490000002</v>
+      </c>
+      <c r="E11" s="14">
+        <v>-23222</v>
+      </c>
+      <c r="F11" s="14">
+        <v>-227522.61490000002</v>
+      </c>
+      <c r="G11" s="15">
+        <v>-227522.62000000002</v>
+      </c>
+      <c r="H11" s="18">
+        <f>F11-G11</f>
+        <v>5.100000009406358E-3</v>
+      </c>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="33">
+        <v>2273843.7274000007</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2093582.8945000002</v>
+      </c>
+      <c r="D12" s="14">
+        <v>43785416.364299983</v>
+      </c>
+      <c r="E12" s="14">
+        <v>2093582.8914999997</v>
+      </c>
+      <c r="F12" s="14">
+        <v>45878999.255799979</v>
+      </c>
+      <c r="G12" s="15">
+        <v>45878999.320000015</v>
+      </c>
+      <c r="H12" s="18">
+        <f>F12-G12</f>
+        <v>-6.4200036227703094E-2</v>
+      </c>
+      <c r="I12" s="40"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="33">
+        <v>4812894.9151000027</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14">
+        <v>91963867.380400062</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="14">
+        <v>91963867.380400062</v>
+      </c>
+      <c r="G13" s="15">
+        <v>91963867.389999986</v>
+      </c>
+      <c r="H13" s="18">
+        <f>F13-G13</f>
+        <v>-9.5999240875244141E-3</v>
+      </c>
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="33">
+        <v>76408.107199999999</v>
+      </c>
+      <c r="C14" s="14">
+        <v>953091.40320000006</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1468530.2485000005</v>
+      </c>
+      <c r="E14" s="14">
+        <v>953091.39999999979</v>
+      </c>
+      <c r="F14" s="14">
+        <v>2421621.6485000001</v>
+      </c>
+      <c r="G14" s="15">
+        <v>2421621.649999999</v>
+      </c>
+      <c r="H14" s="18">
+        <f>F14-G14</f>
+        <v>-1.4999988488852978E-3</v>
+      </c>
+      <c r="I14" s="40"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="33">
+        <v>15693.570400000001</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14">
+        <v>303015.25</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="14">
+        <v>303015.25</v>
+      </c>
+      <c r="G15" s="15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="18">
+        <f>F15-G15</f>
+        <v>303015.25</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="33">
+        <v>6543.9660000000003</v>
+      </c>
+      <c r="C16" s="14">
+        <v>2140154.8114</v>
+      </c>
+      <c r="D16" s="14">
+        <v>122662.45500000002</v>
+      </c>
+      <c r="E16" s="14">
+        <v>2140154.8061999995</v>
+      </c>
+      <c r="F16" s="14">
+        <v>2262817.2611999996</v>
+      </c>
+      <c r="G16" s="15">
+        <v>2262817.2499999991</v>
+      </c>
+      <c r="H16" s="18">
+        <f>F16-G16</f>
+        <v>1.1200000531971455E-2</v>
+      </c>
+      <c r="I16" s="40"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="33">
+        <v>6003.77</v>
+      </c>
+      <c r="C17" s="14">
+        <v>467240.33000000007</v>
+      </c>
+      <c r="D17" s="14">
+        <v>113052.64079999999</v>
+      </c>
+      <c r="E17" s="14">
+        <v>467240.32970000006</v>
+      </c>
+      <c r="F17" s="14">
+        <v>580292.97050000005</v>
+      </c>
+      <c r="G17" s="15">
+        <v>580292.95000000007</v>
+      </c>
+      <c r="H17" s="18">
+        <f>F17-G17</f>
+        <v>2.0499999984167516E-2</v>
+      </c>
+      <c r="I17" s="40"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="14">
+        <v>2282441.5276000001</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="14">
+        <v>2282441.5255999998</v>
+      </c>
+      <c r="F18" s="14">
+        <v>2282441.5255999998</v>
+      </c>
+      <c r="G18" s="15">
+        <v>2282441.52</v>
+      </c>
+      <c r="H18" s="18">
+        <f>F18-G18</f>
+        <v>5.59999980032444E-3</v>
+      </c>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="33">
+        <v>91197.16</v>
+      </c>
+      <c r="C19" s="14">
+        <v>28497266.538799923</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1744491.8740000001</v>
+      </c>
+      <c r="E19" s="14">
+        <v>28497266.525500044</v>
+      </c>
+      <c r="F19" s="14">
+        <v>30241758.399500046</v>
+      </c>
+      <c r="G19" s="15">
+        <v>30074302.809999984</v>
+      </c>
+      <c r="H19" s="18">
+        <f>F19-G19</f>
+        <v>167455.58950006217</v>
+      </c>
+      <c r="I19" s="40"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="33">
+        <v>-4699382.6977000032</v>
+      </c>
+      <c r="C20" s="14">
+        <v>-31340477.586599946</v>
+      </c>
+      <c r="D20" s="14">
+        <v>-87473455.146899983</v>
+      </c>
+      <c r="E20" s="14">
+        <v>-31340477.558600053</v>
+      </c>
+      <c r="F20" s="14">
+        <v>-118813932.70550004</v>
+      </c>
+      <c r="G20" s="15">
+        <v>-118656140.56000003</v>
+      </c>
+      <c r="H20" s="18">
+        <f>F20-G20</f>
+        <v>-157792.14550000429</v>
+      </c>
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="33">
+        <v>0</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14">
+        <v>6961029.4586000061</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="14">
+        <v>6961029.4586000061</v>
+      </c>
+      <c r="G21" s="15">
+        <v>6961029.4400000004</v>
+      </c>
+      <c r="H21" s="18">
+        <f>F21-G21</f>
+        <v>1.8600005656480789E-2</v>
+      </c>
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="33">
+        <v>0</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14">
+        <v>-72995.217700000008</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21">
+        <v>-72995.217700000008</v>
+      </c>
+      <c r="G22" s="22">
+        <v>-72995.209999999992</v>
+      </c>
+      <c r="H22" s="23">
+        <f>F22-G22</f>
+        <v>-7.7000000164844096E-3</v>
+      </c>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="34">
+        <f t="shared" ref="B23:H23" si="0">SUM(B2:B22)</f>
+        <v>9806122.0594000015</v>
+      </c>
+      <c r="C23" s="25">
         <f t="shared" si="0"/>
-        <v>7.0999935269355774E-3</v>
-      </c>
-      <c r="J5" s="44"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="37">
-        <v>-2.4199999978009146E-2</v>
-      </c>
-      <c r="C6" s="17">
-        <v>1.999999993131496E-3</v>
-      </c>
-      <c r="D6" s="17">
-        <v>-206275.19670000148</v>
-      </c>
-      <c r="E6" s="17">
-        <v>1.9000000029336661E-3</v>
-      </c>
-      <c r="F6" s="17">
-        <v>-206275.19480000148</v>
-      </c>
-      <c r="G6" s="18">
-        <v>-189332.92999999996</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="21">
+        <v>32810825.937699974</v>
+      </c>
+      <c r="D23" s="25">
         <f t="shared" si="0"/>
-        <v>-16942.264800001518</v>
-      </c>
-      <c r="J6" s="44"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="37">
-        <v>7534.1304000000009</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17">
-        <v>146948.69279999999</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="17">
-        <v>146948.69279999999</v>
-      </c>
-      <c r="G7" s="18">
-        <v>146948.69</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="21">
+        <v>192464191.37090006</v>
+      </c>
+      <c r="E23" s="25">
         <f t="shared" si="0"/>
-        <v>2.7999999874737114E-3</v>
-      </c>
-      <c r="J7" s="44"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="37">
-        <v>0</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17">
-        <v>0</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="17">
-        <v>0</v>
-      </c>
-      <c r="G8" s="18">
-        <v>0</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="22">
+        <v>32810825.938699991</v>
+      </c>
+      <c r="F23" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="44"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="37">
-        <v>-43798.515700000004</v>
-      </c>
-      <c r="C9" s="17">
-        <v>-3502</v>
-      </c>
-      <c r="D9" s="17">
-        <v>-851206.85509999993</v>
-      </c>
-      <c r="E9" s="17">
-        <v>-3502</v>
-      </c>
-      <c r="F9" s="17">
-        <v>-854708.85509999993</v>
-      </c>
-      <c r="G9" s="18">
-        <v>-715496.49</v>
-      </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="20">
+        <v>225275017.30960011</v>
+      </c>
+      <c r="G23" s="25">
         <f t="shared" si="0"/>
-        <v>-139212.36509999994</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="37">
-        <v>-2336.2399999999998</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17">
-        <v>-44064.056199999999</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="17">
-        <v>-44064.056199999999</v>
-      </c>
-      <c r="G10" s="18">
-        <v>-44064.06</v>
-      </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="21">
+        <v>32590555.289999973</v>
+      </c>
+      <c r="H23" s="47">
         <f t="shared" si="0"/>
-        <v>3.7999999985913746E-3</v>
-      </c>
-      <c r="J10" s="44"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="37">
-        <v>-10301.460000000001</v>
-      </c>
-      <c r="C11" s="17">
-        <v>-23222</v>
-      </c>
-      <c r="D11" s="17">
-        <v>-204300.61490000002</v>
-      </c>
-      <c r="E11" s="17">
-        <v>-23222</v>
-      </c>
-      <c r="F11" s="17">
-        <v>-227522.61490000002</v>
-      </c>
-      <c r="G11" s="18">
-        <v>-227522.62000000002</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="21">
-        <f t="shared" ref="I11:I22" si="1">F11-G11</f>
-        <v>5.100000009406358E-3</v>
-      </c>
-      <c r="J11" s="44"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="37">
-        <v>2273843.7274000007</v>
-      </c>
-      <c r="C12" s="17">
-        <v>2093582.8945000002</v>
-      </c>
-      <c r="D12" s="17">
-        <v>43785416.364299983</v>
-      </c>
-      <c r="E12" s="17">
-        <v>2093582.8914999997</v>
-      </c>
-      <c r="F12" s="17">
-        <v>45878999.255799979</v>
-      </c>
-      <c r="G12" s="18">
-        <v>45878999.320000015</v>
-      </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="21">
-        <f t="shared" si="1"/>
-        <v>-6.4200036227703094E-2</v>
-      </c>
-      <c r="J12" s="44"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="37">
-        <v>4812894.9151000027</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17">
-        <v>91963867.380400062</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="17">
-        <v>91963867.380400062</v>
-      </c>
-      <c r="G13" s="18">
-        <v>91963867.389999986</v>
-      </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="21">
-        <f t="shared" si="1"/>
-        <v>-9.5999240875244141E-3</v>
-      </c>
-      <c r="J13" s="44"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="37">
-        <v>76408.107199999999</v>
-      </c>
-      <c r="C14" s="17">
-        <v>953091.40320000006</v>
-      </c>
-      <c r="D14" s="17">
-        <v>1468530.2485000005</v>
-      </c>
-      <c r="E14" s="17">
-        <v>953091.39999999979</v>
-      </c>
-      <c r="F14" s="17">
-        <v>2421621.6485000001</v>
-      </c>
-      <c r="G14" s="18">
-        <v>2421621.649999999</v>
-      </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="21">
-        <f t="shared" si="1"/>
-        <v>-1.4999988488852978E-3</v>
-      </c>
-      <c r="J14" s="44"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="37">
-        <v>15693.570400000001</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17">
-        <v>303015.25</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="17">
-        <v>303015.25</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="21">
-        <f t="shared" si="1"/>
-        <v>303015.25</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="37">
-        <v>6543.9660000000003</v>
-      </c>
-      <c r="C16" s="17">
-        <v>2140154.8114</v>
-      </c>
-      <c r="D16" s="17">
-        <v>122662.45500000002</v>
-      </c>
-      <c r="E16" s="17">
-        <v>2140154.8061999995</v>
-      </c>
-      <c r="F16" s="17">
-        <v>2262817.2611999996</v>
-      </c>
-      <c r="G16" s="18">
-        <v>2262817.2499999991</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="21">
-        <f t="shared" si="1"/>
-        <v>1.1200000531971455E-2</v>
-      </c>
-      <c r="J16" s="44"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="37">
-        <v>6003.77</v>
-      </c>
-      <c r="C17" s="17">
-        <v>467240.33000000007</v>
-      </c>
-      <c r="D17" s="17">
-        <v>113052.64079999999</v>
-      </c>
-      <c r="E17" s="17">
-        <v>467240.32970000006</v>
-      </c>
-      <c r="F17" s="17">
-        <v>580292.97050000005</v>
-      </c>
-      <c r="G17" s="18">
-        <v>580292.95000000007</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="21">
-        <f t="shared" si="1"/>
-        <v>2.0499999984167516E-2</v>
-      </c>
-      <c r="J17" s="44"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="17">
-        <v>2282441.5276000001</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="17">
-        <v>2282441.5255999998</v>
-      </c>
-      <c r="F18" s="17">
-        <v>2282441.5255999998</v>
-      </c>
-      <c r="G18" s="18">
-        <v>2282441.52</v>
-      </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="21">
-        <f t="shared" si="1"/>
-        <v>5.59999980032444E-3</v>
-      </c>
-      <c r="J18" s="44"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+        <v>156519.32960009674</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="37">
-        <v>91197.16</v>
-      </c>
-      <c r="C19" s="17">
-        <v>28497266.538799923</v>
-      </c>
-      <c r="D19" s="17">
-        <v>1744491.8740000001</v>
-      </c>
-      <c r="E19" s="17">
-        <v>28497266.525500044</v>
-      </c>
-      <c r="F19" s="17">
-        <v>30241758.399500046</v>
-      </c>
-      <c r="G19" s="18">
-        <v>30074302.809999984</v>
-      </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="21">
-        <f t="shared" si="1"/>
-        <v>167455.58950006217</v>
-      </c>
-      <c r="J19" s="44"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="37">
-        <v>-4699382.6977000032</v>
-      </c>
-      <c r="C20" s="17">
-        <v>-31340477.586599946</v>
-      </c>
-      <c r="D20" s="17">
-        <v>-87473455.146899983</v>
-      </c>
-      <c r="E20" s="17">
-        <v>-31340477.558600053</v>
-      </c>
-      <c r="F20" s="17">
-        <v>-118813932.70550004</v>
-      </c>
-      <c r="G20" s="18">
-        <v>-118656140.56000003</v>
-      </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="21">
-        <f t="shared" si="1"/>
-        <v>-157792.14550000429</v>
-      </c>
-      <c r="J20" s="44"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="37">
-        <v>0</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
-        <v>6961029.4586000061</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="17">
-        <v>6961029.4586000061</v>
-      </c>
-      <c r="G21" s="18">
-        <v>6961029.4400000004</v>
-      </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="21">
-        <f t="shared" si="1"/>
-        <v>1.8600005656480789E-2</v>
-      </c>
-      <c r="J21" s="44"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="37">
-        <v>0</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
-        <v>-72995.217700000008</v>
-      </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24">
-        <v>-72995.217700000008</v>
-      </c>
-      <c r="G22" s="25">
-        <v>-72995.209999999992</v>
-      </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="26">
-        <f t="shared" si="1"/>
-        <v>-7.7000000164844096E-3</v>
-      </c>
-      <c r="J22" s="44"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="38">
-        <f t="shared" ref="B23:I23" si="2">SUM(B2:B22)</f>
-        <v>9806122.0594000015</v>
-      </c>
-      <c r="C23" s="28">
-        <f t="shared" si="2"/>
-        <v>32810825.937699974</v>
-      </c>
-      <c r="D23" s="28">
-        <f t="shared" si="2"/>
-        <v>192464191.37090006</v>
-      </c>
-      <c r="E23" s="28">
-        <f t="shared" si="2"/>
-        <v>32810825.938699991</v>
-      </c>
-      <c r="F23" s="28">
-        <f t="shared" si="2"/>
-        <v>225275017.30960011</v>
-      </c>
-      <c r="G23" s="28">
-        <f t="shared" si="2"/>
-        <v>32590555.289999973</v>
-      </c>
-      <c r="H23" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="52">
-        <f t="shared" si="2"/>
-        <v>156519.32960009674</v>
-      </c>
-      <c r="J23" s="43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="39">
+      <c r="B24" s="35">
         <v>9805347.0899999999</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="27">
         <v>32806116.399999999</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="27">
         <v>192473715.09999999</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="27">
         <v>32806116.399999999</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="28">
         <f>D24+E24</f>
         <v>225279831.5</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="31">
         <f>B24-B23</f>
         <v>-774.96940000168979</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="31">
         <f>C24-C23</f>
         <v>-4709.5376999750733</v>
       </c>
-      <c r="D25" s="35">
-        <f t="shared" ref="D25:F25" si="3">D24-D23</f>
+      <c r="D25" s="31">
+        <f t="shared" ref="D25:F25" si="1">D24-D23</f>
         <v>9523.7290999293327</v>
       </c>
-      <c r="E25" s="35">
-        <f t="shared" si="3"/>
+      <c r="E25" s="31">
+        <f t="shared" si="1"/>
         <v>-4709.5386999920011</v>
       </c>
-      <c r="F25" s="35">
-        <f t="shared" si="3"/>
+      <c r="F25" s="31">
+        <f t="shared" si="1"/>
         <v>4814.1903998851776</v>
       </c>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51" t="s">
-        <v>36</v>
+      <c r="G25" s="44"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualualiza ejemplos Caratula con saldos iniciales del sistema
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>concepto</t>
   </si>
@@ -122,17 +122,18 @@
   </si>
   <si>
     <t>Total Cartera</t>
+  </si>
+  <si>
+    <t>Saldo Inicial Esperado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
-    <numFmt numFmtId="165" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -234,18 +235,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -419,17 +420,6 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -511,146 +501,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="40" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,15 +548,130 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="9" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -974,689 +979,715 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="36" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73" style="41" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.42578125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="51"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="32">
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="51">
         <v>8867057.4600000009</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="52">
         <v>27863597.690000001</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="52">
         <v>164664345</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="52">
         <v>27863597.690000001</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="53">
         <f>D3+E3</f>
         <v>192527942.69</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="42" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
+    </row>
+    <row r="4" spans="1:9" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="26">
+        <v>8866283.2861000001</v>
+      </c>
+      <c r="C4" s="27">
+        <v>27858891.291499998</v>
+      </c>
+      <c r="D4" s="27">
+        <v>164711604.49086601</v>
+      </c>
+      <c r="E4" s="27">
+        <v>27858891.291500099</v>
+      </c>
+      <c r="F4" s="28">
+        <f>D4+E4</f>
+        <v>192570495.7823661</v>
+      </c>
+      <c r="G4" s="29">
+        <v>192527942.97</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B5" s="31">
         <v>-0.11949999999999997</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C5" s="32">
         <v>-1.32E-2</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D5" s="32">
         <v>-2.2530000000000006</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E5" s="33">
         <v>-1.32E-2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F5" s="32">
         <v>-2.2662000000000004</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G5" s="33">
         <v>2.46</v>
       </c>
-      <c r="H4" s="17">
-        <f>F4-G4</f>
+      <c r="H5" s="34">
+        <f t="shared" ref="H5:H23" si="0">F5-G5</f>
         <v>-4.7262000000000004</v>
       </c>
-      <c r="I4" s="40"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B6" s="31">
         <v>-1595235.69</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C6" s="32">
         <v>-119347.66</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D6" s="32">
         <v>-29956868.653000001</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E6" s="33">
         <v>-119347.6599</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F6" s="32">
         <v>-30076216.312899999</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G6" s="33">
         <v>-30076216.319999993</v>
       </c>
-      <c r="H5" s="18">
-        <f>F5-G5</f>
+      <c r="H6" s="34">
+        <f t="shared" si="0"/>
         <v>7.0999935269355774E-3</v>
       </c>
-      <c r="I5" s="40"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B7" s="31">
         <v>-2.4199999978009146E-2</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C7" s="32">
         <v>1.999999993131496E-3</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D7" s="32">
         <v>-206275.19670000148</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E7" s="33">
         <v>1.9000000029336661E-3</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F7" s="32">
         <v>-206275.19480000148</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G7" s="33">
         <v>-189332.92999999996</v>
       </c>
-      <c r="H6" s="18">
-        <f>F6-G6</f>
+      <c r="H7" s="34">
+        <f t="shared" si="0"/>
         <v>-16942.264800001518</v>
       </c>
-      <c r="I6" s="40"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B8" s="31">
         <v>7534.1304000000009</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14">
+      <c r="C8" s="32"/>
+      <c r="D8" s="32">
         <v>146948.69279999999</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="14">
+      <c r="E8" s="33"/>
+      <c r="F8" s="32">
         <v>146948.69279999999</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G8" s="33">
         <v>146948.69</v>
       </c>
-      <c r="H7" s="18">
-        <f>F7-G7</f>
+      <c r="H8" s="34">
+        <f t="shared" si="0"/>
         <v>2.7999999874737114E-3</v>
       </c>
-      <c r="I7" s="40"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B9" s="31">
         <v>0</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32">
         <v>0</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="14">
+      <c r="E9" s="33"/>
+      <c r="F9" s="32">
         <v>0</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G9" s="33">
         <v>0</v>
       </c>
-      <c r="H8" s="19">
-        <f>F8-G8</f>
+      <c r="H9" s="34">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="40"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B10" s="31">
         <v>-43798.515700000004</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C10" s="32">
         <v>-3502</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D10" s="32">
         <v>-851206.85509999993</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E10" s="33">
         <v>-3502</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F10" s="32">
         <v>-854708.85509999993</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G10" s="33">
         <v>-715496.49</v>
       </c>
-      <c r="H9" s="17">
-        <f>F9-G9</f>
+      <c r="H10" s="34">
+        <f t="shared" si="0"/>
         <v>-139212.36509999994</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B11" s="31">
         <v>-2336.2399999999998</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32">
         <v>-44064.056199999999</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="14">
+      <c r="E11" s="33"/>
+      <c r="F11" s="32">
         <v>-44064.056199999999</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G11" s="33">
         <v>-44064.06</v>
       </c>
-      <c r="H10" s="18">
-        <f>F10-G10</f>
+      <c r="H11" s="34">
+        <f t="shared" si="0"/>
         <v>3.7999999985913746E-3</v>
       </c>
-      <c r="I10" s="40"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B12" s="31">
         <v>-10301.460000000001</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C12" s="32">
         <v>-23222</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D12" s="32">
         <v>-204300.61490000002</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E12" s="33">
         <v>-23222</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F12" s="32">
         <v>-227522.61490000002</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G12" s="33">
         <v>-227522.62000000002</v>
       </c>
-      <c r="H11" s="18">
-        <f>F11-G11</f>
+      <c r="H12" s="34">
+        <f t="shared" si="0"/>
         <v>5.100000009406358E-3</v>
       </c>
-      <c r="I11" s="40"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B13" s="31">
         <v>2273843.7274000007</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C13" s="32">
         <v>2093582.8945000002</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D13" s="32">
         <v>43785416.364299983</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E13" s="33">
         <v>2093582.8914999997</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F13" s="32">
         <v>45878999.255799979</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G13" s="33">
         <v>45878999.320000015</v>
       </c>
-      <c r="H12" s="18">
-        <f>F12-G12</f>
+      <c r="H13" s="34">
+        <f t="shared" si="0"/>
         <v>-6.4200036227703094E-2</v>
       </c>
-      <c r="I12" s="40"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B14" s="31">
         <v>4812894.9151000027</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32">
         <v>91963867.380400062</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="14">
+      <c r="E14" s="33"/>
+      <c r="F14" s="32">
         <v>91963867.380400062</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G14" s="33">
         <v>91963867.389999986</v>
       </c>
-      <c r="H13" s="18">
-        <f>F13-G13</f>
+      <c r="H14" s="34">
+        <f t="shared" si="0"/>
         <v>-9.5999240875244141E-3</v>
       </c>
-      <c r="I13" s="40"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B15" s="31">
         <v>76408.107199999999</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C15" s="32">
         <v>953091.40320000006</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D15" s="32">
         <v>1468530.2485000005</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E15" s="33">
         <v>953091.39999999979</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F15" s="32">
         <v>2421621.6485000001</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G15" s="33">
         <v>2421621.649999999</v>
       </c>
-      <c r="H14" s="18">
-        <f>F14-G14</f>
+      <c r="H15" s="34">
+        <f t="shared" si="0"/>
         <v>-1.4999988488852978E-3</v>
       </c>
-      <c r="I14" s="40"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B16" s="31">
         <v>15693.570400000001</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32">
         <v>303015.25</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="14">
+      <c r="E16" s="33"/>
+      <c r="F16" s="32">
         <v>303015.25</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G16" s="33">
         <v>0</v>
       </c>
-      <c r="H15" s="18">
-        <f>F15-G15</f>
+      <c r="H16" s="34">
+        <f t="shared" si="0"/>
         <v>303015.25</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B17" s="31">
         <v>6543.9660000000003</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C17" s="32">
         <v>2140154.8114</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D17" s="32">
         <v>122662.45500000002</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E17" s="33">
         <v>2140154.8061999995</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F17" s="32">
         <v>2262817.2611999996</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G17" s="33">
         <v>2262817.2499999991</v>
       </c>
-      <c r="H16" s="18">
-        <f>F16-G16</f>
+      <c r="H17" s="34">
+        <f t="shared" si="0"/>
         <v>1.1200000531971455E-2</v>
       </c>
-      <c r="I16" s="40"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B18" s="31">
         <v>6003.77</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C18" s="32">
         <v>467240.33000000007</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D18" s="32">
         <v>113052.64079999999</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E18" s="33">
         <v>467240.32970000006</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F18" s="32">
         <v>580292.97050000005</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G18" s="33">
         <v>580292.95000000007</v>
       </c>
-      <c r="H17" s="18">
-        <f>F17-G17</f>
+      <c r="H18" s="34">
+        <f t="shared" si="0"/>
         <v>2.0499999984167516E-2</v>
       </c>
-      <c r="I17" s="40"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="14">
+      <c r="B19" s="31"/>
+      <c r="C19" s="32">
         <v>2282441.5276000001</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="14">
+      <c r="D19" s="32"/>
+      <c r="E19" s="33">
         <v>2282441.5255999998</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F19" s="32">
         <v>2282441.5255999998</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G19" s="33">
         <v>2282441.52</v>
       </c>
-      <c r="H18" s="18">
-        <f>F18-G18</f>
+      <c r="H19" s="34">
+        <f t="shared" si="0"/>
         <v>5.59999980032444E-3</v>
       </c>
-      <c r="I18" s="40"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B20" s="31">
         <v>91197.16</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C20" s="32">
         <v>28497266.538799923</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D20" s="32">
         <v>1744491.8740000001</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E20" s="33">
         <v>28497266.525500044</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F20" s="32">
         <v>30241758.399500046</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G20" s="33">
         <v>30074302.809999984</v>
       </c>
-      <c r="H19" s="18">
-        <f>F19-G19</f>
+      <c r="H20" s="34">
+        <f t="shared" si="0"/>
         <v>167455.58950006217</v>
       </c>
-      <c r="I19" s="40"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B21" s="31">
         <v>-4699382.6977000032</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C21" s="32">
         <v>-31340477.586599946</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D21" s="32">
         <v>-87473455.146899983</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E21" s="33">
         <v>-31340477.558600053</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F21" s="32">
         <v>-118813932.70550004</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G21" s="33">
         <v>-118656140.56000003</v>
       </c>
-      <c r="H20" s="18">
-        <f>F20-G20</f>
+      <c r="H21" s="34">
+        <f t="shared" si="0"/>
         <v>-157792.14550000429</v>
       </c>
-      <c r="I20" s="40"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B22" s="31">
         <v>0</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32">
         <v>6961029.4586000061</v>
       </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="14">
+      <c r="E22" s="33"/>
+      <c r="F22" s="32">
         <v>6961029.4586000061</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G22" s="33">
         <v>6961029.4400000004</v>
       </c>
-      <c r="H21" s="18">
-        <f>F21-G21</f>
+      <c r="H22" s="34">
+        <f t="shared" si="0"/>
         <v>1.8600005656480789E-2</v>
       </c>
-      <c r="I21" s="40"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B23" s="31">
         <v>0</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32">
         <v>-72995.217700000008</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21">
+      <c r="E23" s="35"/>
+      <c r="F23" s="36">
         <v>-72995.217700000008</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G23" s="35">
         <v>-72995.209999999992</v>
       </c>
-      <c r="H22" s="23">
-        <f>F22-G22</f>
+      <c r="H23" s="37">
+        <f t="shared" si="0"/>
         <v>-7.7000000164844096E-3</v>
       </c>
-      <c r="I22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="34">
-        <f t="shared" ref="B23:H23" si="0">SUM(B2:B22)</f>
-        <v>9806122.0594000015</v>
-      </c>
-      <c r="C23" s="25">
-        <f t="shared" si="0"/>
-        <v>32810825.937699974</v>
-      </c>
-      <c r="D23" s="25">
-        <f t="shared" si="0"/>
-        <v>192464191.37090006</v>
-      </c>
-      <c r="E23" s="25">
-        <f t="shared" si="0"/>
-        <v>32810825.938699991</v>
-      </c>
-      <c r="F23" s="25">
-        <f t="shared" si="0"/>
-        <v>225275017.30960011</v>
-      </c>
-      <c r="G23" s="25">
-        <f t="shared" si="0"/>
-        <v>32590555.289999973</v>
-      </c>
-      <c r="H23" s="47">
-        <f t="shared" si="0"/>
-        <v>156519.32960009674</v>
-      </c>
-      <c r="I23" s="39" t="s">
+      <c r="B24" s="38">
+        <f>SUM(B4:B23)</f>
+        <v>9805347.8855000008</v>
+      </c>
+      <c r="C24" s="38">
+        <f t="shared" ref="C24:H24" si="1">SUM(C4:C23)</f>
+        <v>32806119.539199978</v>
+      </c>
+      <c r="D24" s="38">
+        <f t="shared" si="1"/>
+        <v>192511450.86176601</v>
+      </c>
+      <c r="E24" s="39">
+        <f t="shared" si="1"/>
+        <v>32806119.540200092</v>
+      </c>
+      <c r="F24" s="38">
+        <f t="shared" si="1"/>
+        <v>225317570.40196621</v>
+      </c>
+      <c r="G24" s="38">
+        <f>SUM(G4:G23)</f>
+        <v>225118498.25999987</v>
+      </c>
+      <c r="H24" s="38">
+        <f>F24-G24</f>
+        <v>199072.14196634293</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B25" s="40">
         <v>9805347.0899999999</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C25" s="41">
         <v>32806116.399999999</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D25" s="41">
         <v>192473715.09999999</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E25" s="41">
         <v>32806116.399999999</v>
       </c>
-      <c r="F24" s="28">
-        <f>D24+E24</f>
+      <c r="F25" s="42">
+        <f>D25+E25</f>
         <v>225279831.5</v>
       </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="42" t="s">
+      <c r="G25" s="41"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="43" t="s">
+    <row r="26" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="31">
-        <f>B24-B23</f>
-        <v>-774.96940000168979</v>
-      </c>
-      <c r="C25" s="31">
-        <f>C24-C23</f>
-        <v>-4709.5376999750733</v>
-      </c>
-      <c r="D25" s="31">
-        <f t="shared" ref="D25:F25" si="1">D24-D23</f>
-        <v>9523.7290999293327</v>
-      </c>
-      <c r="E25" s="31">
-        <f t="shared" si="1"/>
-        <v>-4709.5386999920011</v>
-      </c>
-      <c r="F25" s="31">
-        <f t="shared" si="1"/>
-        <v>4814.1903998851776</v>
-      </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46" t="s">
+      <c r="B26" s="44">
+        <f>B25-B24</f>
+        <v>-0.79550000093877316</v>
+      </c>
+      <c r="C26" s="44">
+        <f>C25-C24</f>
+        <v>-3.1391999796032906</v>
+      </c>
+      <c r="D26" s="44">
+        <f t="shared" ref="D26:F26" si="2">D25-D24</f>
+        <v>-37735.761766016483</v>
+      </c>
+      <c r="E26" s="45">
+        <f t="shared" si="2"/>
+        <v>-3.1402000933885574</v>
+      </c>
+      <c r="F26" s="44">
+        <f t="shared" si="2"/>
+        <v>-37738.90196621418</v>
+      </c>
+      <c r="G26" s="45"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="13" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se añade renglon de Polizas contables a la caratula
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>concepto</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Saldo Final Intranet</t>
+  </si>
+  <si>
+    <t>Polizas Manuales</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,8 +272,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -680,20 +689,131 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -706,9 +826,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -722,18 +840,7 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -744,18 +851,35 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -768,35 +892,48 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -804,7 +941,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -826,13 +963,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -840,21 +971,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,6 +984,147 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="14" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -877,200 +1137,104 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="3" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="12" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="14" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="18" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="3" fillId="12" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="3" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1380,13 +1544,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" sqref="A1:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,675 +1562,675 @@
     <col min="5" max="5" width="14.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="79.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="29" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="70" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="37"/>
-    </row>
-    <row r="3" spans="1:9" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="I2" s="71"/>
+    </row>
+    <row r="3" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="73">
         <v>8867057.4600000009</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="74">
         <v>27863597.690000001</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="27">
         <v>164664345</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="27">
         <v>27863597.690000001</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="28">
         <f>D3+E3</f>
         <v>192527942.69</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="29">
         <v>192527942.97</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="30">
         <f>F3-G3</f>
         <v>-0.2800000011920929</v>
       </c>
-      <c r="I3" s="45"/>
-    </row>
-    <row r="4" spans="1:9" s="25" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="I3" s="31"/>
+    </row>
+    <row r="4" spans="1:9" s="19" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="75">
         <v>8866283.2861000001</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="33">
         <v>27858891.291499998</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="35">
         <v>164664345</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="34">
         <v>27858891.291500099</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="36">
         <f>D4+E4</f>
         <v>192523236.29150009</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="37">
         <v>192527942.97</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="38">
         <f>F4-G4</f>
         <v>-4706.6784999072552</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+    <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="76">
         <v>-0.11949999999999997</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="41">
         <v>-1.32E-2</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>-2.2530000000000006</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="42">
         <v>-1.32E-2</v>
       </c>
-      <c r="F5" s="56">
+      <c r="F5" s="41">
         <v>-2.2662000000000004</v>
       </c>
-      <c r="G5" s="57">
+      <c r="G5" s="42">
         <v>2.46</v>
       </c>
-      <c r="H5" s="58">
+      <c r="H5" s="77">
         <f t="shared" ref="H5:H23" si="0">F5-G5</f>
         <v>-4.7262000000000004</v>
       </c>
-      <c r="I5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="I5" s="43"/>
+    </row>
+    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="78">
         <v>-1595235.69</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="45">
         <v>-119347.66</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>-29956868.653000001</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="46">
         <v>-119347.6599</v>
       </c>
-      <c r="F6" s="61">
+      <c r="F6" s="45">
         <v>-30076216.312899999</v>
       </c>
-      <c r="G6" s="62">
+      <c r="G6" s="46">
         <v>-30076216.319999993</v>
       </c>
-      <c r="H6" s="63">
+      <c r="H6" s="79">
         <f t="shared" si="0"/>
         <v>7.0999935269355774E-3</v>
       </c>
-      <c r="I6" s="64"/>
-    </row>
-    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="I6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="78">
         <v>-2.4199999978009146E-2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="45">
         <v>1.999999993131496E-3</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>-206275.19670000148</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="46">
         <v>1.9000000029336661E-3</v>
       </c>
-      <c r="F7" s="61">
+      <c r="F7" s="45">
         <v>-206275.19480000148</v>
       </c>
-      <c r="G7" s="62">
+      <c r="G7" s="46">
         <v>-189332.92999999996</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="79">
         <f t="shared" si="0"/>
         <v>-16942.264800001518</v>
       </c>
-      <c r="I7" s="64"/>
-    </row>
-    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="I7" s="47"/>
+    </row>
+    <row r="8" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="78">
         <v>7534.1304000000009</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9">
+      <c r="C8" s="45"/>
+      <c r="D8" s="8">
         <v>146948.69279999999</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="61">
+      <c r="E8" s="46"/>
+      <c r="F8" s="45">
         <v>146948.69279999999</v>
       </c>
-      <c r="G8" s="62">
+      <c r="G8" s="46">
         <v>146948.69</v>
       </c>
-      <c r="H8" s="63">
+      <c r="H8" s="79">
         <f t="shared" si="0"/>
         <v>2.7999999874737114E-3</v>
       </c>
-      <c r="I8" s="64"/>
-    </row>
-    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="I8" s="47"/>
+    </row>
+    <row r="9" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="78">
         <v>0</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9">
+      <c r="C9" s="45"/>
+      <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="61">
+      <c r="E9" s="46"/>
+      <c r="F9" s="45">
         <v>0</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="46">
         <v>0</v>
       </c>
-      <c r="H9" s="63">
+      <c r="H9" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="64"/>
-    </row>
-    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
+      <c r="I9" s="47"/>
+    </row>
+    <row r="10" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="78">
         <v>-43798.515700000004</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="45">
         <v>-3502</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>-851206.85509999993</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="46">
         <v>-3502</v>
       </c>
-      <c r="F10" s="61">
+      <c r="F10" s="45">
         <v>-854708.85509999993</v>
       </c>
-      <c r="G10" s="62">
+      <c r="G10" s="46">
         <v>-715496.49</v>
       </c>
-      <c r="H10" s="63">
+      <c r="H10" s="79">
         <f t="shared" si="0"/>
         <v>-139212.36509999994</v>
       </c>
-      <c r="I10" s="65" t="s">
+      <c r="I10" s="48" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+    <row r="11" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="78">
         <v>-2336.2399999999998</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9">
+      <c r="C11" s="45"/>
+      <c r="D11" s="8">
         <v>-44064.056199999999</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="61">
+      <c r="E11" s="46"/>
+      <c r="F11" s="45">
         <v>-44064.056199999999</v>
       </c>
-      <c r="G11" s="62">
+      <c r="G11" s="46">
         <v>-44064.06</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="79">
         <f t="shared" si="0"/>
         <v>3.7999999985913746E-3</v>
       </c>
-      <c r="I11" s="64"/>
-    </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="I11" s="47"/>
+    </row>
+    <row r="12" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="78">
         <v>-10301.460000000001</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="45">
         <v>-23222</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>-204300.61490000002</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="46">
         <v>-23222</v>
       </c>
-      <c r="F12" s="61">
+      <c r="F12" s="45">
         <v>-227522.61490000002</v>
       </c>
-      <c r="G12" s="62">
+      <c r="G12" s="46">
         <v>-227522.62000000002</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="79">
         <f t="shared" si="0"/>
         <v>5.100000009406358E-3</v>
       </c>
-      <c r="I12" s="64"/>
-    </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
+      <c r="I12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="78">
         <v>2273843.7274000007</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="45">
         <v>2093582.8945000002</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>43785416.364299983</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="46">
         <v>2093582.8914999997</v>
       </c>
-      <c r="F13" s="61">
+      <c r="F13" s="45">
         <v>45878999.255799979</v>
       </c>
-      <c r="G13" s="62">
+      <c r="G13" s="46">
         <v>45878999.320000015</v>
       </c>
-      <c r="H13" s="63">
+      <c r="H13" s="79">
         <f t="shared" si="0"/>
         <v>-6.4200036227703094E-2</v>
       </c>
-      <c r="I13" s="64"/>
-    </row>
-    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="I13" s="47"/>
+    </row>
+    <row r="14" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="78">
         <v>4812894.9151000027</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9">
+      <c r="C14" s="45"/>
+      <c r="D14" s="8">
         <v>91963867.380400062</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="61">
+      <c r="E14" s="46"/>
+      <c r="F14" s="45">
         <v>91963867.380400062</v>
       </c>
-      <c r="G14" s="62">
+      <c r="G14" s="46">
         <v>91963867.389999986</v>
       </c>
-      <c r="H14" s="63">
+      <c r="H14" s="79">
         <f t="shared" si="0"/>
         <v>-9.5999240875244141E-3</v>
       </c>
-      <c r="I14" s="64"/>
-    </row>
-    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="I14" s="47"/>
+    </row>
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="78">
         <v>76408.107199999999</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="45">
         <v>953091.40320000006</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>1468530.2485000005</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="46">
         <v>953091.39999999979</v>
       </c>
-      <c r="F15" s="61">
+      <c r="F15" s="45">
         <v>2421621.6485000001</v>
       </c>
-      <c r="G15" s="62">
+      <c r="G15" s="46">
         <v>2421621.649999999</v>
       </c>
-      <c r="H15" s="63">
+      <c r="H15" s="79">
         <f t="shared" si="0"/>
         <v>-1.4999988488852978E-3</v>
       </c>
-      <c r="I15" s="64"/>
-    </row>
-    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="I15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="78">
         <v>15693.570400000001</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9">
+      <c r="C16" s="45"/>
+      <c r="D16" s="8">
         <v>303015.25</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="61">
+      <c r="E16" s="46"/>
+      <c r="F16" s="45">
         <v>303015.25</v>
       </c>
-      <c r="G16" s="62">
+      <c r="G16" s="46">
         <v>0</v>
       </c>
-      <c r="H16" s="63">
+      <c r="H16" s="79">
         <f t="shared" si="0"/>
         <v>303015.25</v>
       </c>
-      <c r="I16" s="65" t="s">
+      <c r="I16" s="48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="78">
         <v>6543.9660000000003</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="45">
         <v>2140154.8114</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>122662.45500000002</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="46">
         <v>2140154.8061999995</v>
       </c>
-      <c r="F17" s="61">
+      <c r="F17" s="45">
         <v>2262817.2611999996</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="46">
         <v>2262817.2499999991</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H17" s="79">
         <f t="shared" si="0"/>
         <v>1.1200000531971455E-2</v>
       </c>
-      <c r="I17" s="64"/>
-    </row>
-    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="I17" s="47"/>
+    </row>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="78">
         <v>6003.77</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="45">
         <v>467240.33000000007</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>113052.64079999999</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="46">
         <v>467240.32970000006</v>
       </c>
-      <c r="F18" s="61">
+      <c r="F18" s="45">
         <v>580292.97050000005</v>
       </c>
-      <c r="G18" s="62">
+      <c r="G18" s="46">
         <v>580292.95000000007</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="79">
         <f t="shared" si="0"/>
         <v>2.0499999984167516E-2</v>
       </c>
-      <c r="I18" s="64"/>
-    </row>
-    <row r="19" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="I18" s="47"/>
+    </row>
+    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9">
+      <c r="B19" s="78"/>
+      <c r="C19" s="45">
         <v>2282441.5276000001</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="18">
+      <c r="D19" s="8"/>
+      <c r="E19" s="46">
         <v>2282441.5255999998</v>
       </c>
-      <c r="F19" s="61">
+      <c r="F19" s="45">
         <v>2282441.5255999998</v>
       </c>
-      <c r="G19" s="62">
+      <c r="G19" s="46">
         <v>2282441.52</v>
       </c>
-      <c r="H19" s="63">
+      <c r="H19" s="79">
         <f t="shared" si="0"/>
         <v>5.59999980032444E-3</v>
       </c>
-      <c r="I19" s="64"/>
-    </row>
-    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="I19" s="47"/>
+    </row>
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="78">
         <v>91197.16</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="45">
         <v>28497266.538799923</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>1744491.8740000001</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="46">
         <v>28497266.525500044</v>
       </c>
-      <c r="F20" s="61">
+      <c r="F20" s="45">
         <v>30241758.399500046</v>
       </c>
-      <c r="G20" s="62">
+      <c r="G20" s="46">
         <v>30074302.809999984</v>
       </c>
-      <c r="H20" s="63">
+      <c r="H20" s="79">
         <f t="shared" si="0"/>
         <v>167455.58950006217</v>
       </c>
-      <c r="I20" s="64"/>
-    </row>
-    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
+      <c r="I20" s="47"/>
+    </row>
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="78">
         <v>-4699382.6977000032</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="45">
         <v>-31340477.586599946</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>-87473455.146899983</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="46">
         <v>-31340477.558600053</v>
       </c>
-      <c r="F21" s="61">
+      <c r="F21" s="45">
         <v>-118813932.70550004</v>
       </c>
-      <c r="G21" s="62">
+      <c r="G21" s="46">
         <v>-118656140.56000003</v>
       </c>
-      <c r="H21" s="63">
+      <c r="H21" s="79">
         <f t="shared" si="0"/>
         <v>-157792.14550000429</v>
       </c>
-      <c r="I21" s="64"/>
-    </row>
-    <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
+      <c r="I21" s="47"/>
+    </row>
+    <row r="22" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="78">
         <v>0</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9">
+      <c r="C22" s="45"/>
+      <c r="D22" s="8">
         <v>6961029.4586000061</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="61">
+      <c r="E22" s="46"/>
+      <c r="F22" s="45">
         <v>6961029.4586000061</v>
       </c>
-      <c r="G22" s="62">
+      <c r="G22" s="46">
         <v>6961029.4400000004</v>
       </c>
-      <c r="H22" s="63">
+      <c r="H22" s="79">
         <f t="shared" si="0"/>
         <v>1.8600005656480789E-2</v>
       </c>
-      <c r="I22" s="64"/>
-    </row>
-    <row r="23" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="I22" s="47"/>
+    </row>
+    <row r="23" spans="1:9" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="80">
         <v>0</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15">
+      <c r="C23" s="50"/>
+      <c r="D23" s="12">
         <v>-72995.217700000008</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="67">
+      <c r="E23" s="51"/>
+      <c r="F23" s="50">
         <v>-72995.217700000008</v>
       </c>
-      <c r="G23" s="68">
+      <c r="G23" s="51">
         <v>-72995.209999999992</v>
       </c>
-      <c r="H23" s="69">
+      <c r="H23" s="81">
         <f t="shared" si="0"/>
         <v>-7.7000000164844096E-3</v>
       </c>
-      <c r="I23" s="70"/>
+      <c r="I23" s="52"/>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="72">
+      <c r="B24" s="55">
         <f>SUM(B5:B23)</f>
         <v>939064.59939999972</v>
       </c>
-      <c r="C24" s="72">
+      <c r="C24" s="56">
         <f t="shared" ref="C24:H24" si="1">SUM(C5:C23)</f>
         <v>4947228.247699976</v>
       </c>
-      <c r="D24" s="72">
+      <c r="D24" s="54">
         <f t="shared" si="1"/>
         <v>27799846.370900061</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="57">
         <f t="shared" si="1"/>
         <v>4947228.2486999929</v>
       </c>
-      <c r="F24" s="74">
+      <c r="F24" s="56">
         <f t="shared" si="1"/>
         <v>32747074.619600054</v>
       </c>
-      <c r="G24" s="75">
-        <f t="shared" si="1"/>
+      <c r="G24" s="57">
+        <f>SUM(G5:G23)</f>
         <v>32590555.289999973</v>
       </c>
-      <c r="H24" s="76">
+      <c r="H24" s="82">
         <f t="shared" si="1"/>
         <v>156519.32960009674</v>
       </c>
-      <c r="I24" s="77"/>
-    </row>
-    <row r="25" spans="1:9" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="78" t="s">
+      <c r="I24" s="58"/>
+    </row>
+    <row r="25" spans="1:9" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="79">
+      <c r="B25" s="61">
         <f t="shared" ref="B25:H25" si="2">B4+B24</f>
         <v>9805347.8854999989</v>
       </c>
-      <c r="C25" s="79">
+      <c r="C25" s="62">
         <f t="shared" si="2"/>
         <v>32806119.539199974</v>
       </c>
-      <c r="D25" s="79">
+      <c r="D25" s="60">
         <f t="shared" si="2"/>
         <v>192464191.37090006</v>
       </c>
-      <c r="E25" s="80">
+      <c r="E25" s="63">
         <f t="shared" si="2"/>
         <v>32806119.540200092</v>
       </c>
-      <c r="F25" s="81">
+      <c r="F25" s="62">
         <f t="shared" si="2"/>
         <v>225270310.91110015</v>
       </c>
-      <c r="G25" s="82">
+      <c r="G25" s="63">
         <f t="shared" si="2"/>
         <v>225118498.25999996</v>
       </c>
@@ -2076,63 +2240,86 @@
       </c>
       <c r="I25" s="84"/>
     </row>
-    <row r="26" spans="1:9" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="90">
+        <v>161333.24</v>
+      </c>
+      <c r="H26" s="91"/>
+      <c r="I26" s="92"/>
+    </row>
+    <row r="27" spans="1:9" s="17" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="86">
+      <c r="B27" s="94">
         <f>B3+B24</f>
         <v>9806122.0593999997</v>
       </c>
-      <c r="C26" s="86">
+      <c r="C27" s="95">
         <f>C3+C24</f>
         <v>32810825.937699977</v>
       </c>
-      <c r="D26" s="86">
+      <c r="D27" s="96">
         <f>D3+D24</f>
         <v>192464191.37090006</v>
       </c>
-      <c r="E26" s="86">
+      <c r="E27" s="97">
         <f>E3+E24</f>
         <v>32810825.938699994</v>
       </c>
-      <c r="F26" s="86">
+      <c r="F27" s="95">
         <f>F3+F24</f>
         <v>225275017.30960006</v>
       </c>
-      <c r="G26" s="87"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="89" t="s">
+      <c r="G27" s="98">
+        <v>225279831.5</v>
+      </c>
+      <c r="H27" s="99">
+        <f>F27-G27</f>
+        <v>-4814.1903999447823</v>
+      </c>
+      <c r="I27" s="100" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="23" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="90" t="s">
+    <row r="28" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="91">
-        <f>B25-B26</f>
+      <c r="B28" s="101">
+        <f>B25-B27</f>
         <v>-774.17390000075102</v>
       </c>
-      <c r="C27" s="91">
-        <f>C25-C26</f>
+      <c r="C28" s="102">
+        <f>(C25+C26)-C27</f>
         <v>-4706.3985000029206</v>
       </c>
-      <c r="D27" s="91">
-        <f>D25-D26</f>
+      <c r="D28" s="65">
+        <f>(D25+D26)-D27</f>
         <v>0</v>
       </c>
-      <c r="E27" s="91">
-        <f>E25-E26</f>
+      <c r="E28" s="65">
+        <f>(E25+E26)-E27</f>
         <v>-4706.3984999023378</v>
       </c>
-      <c r="F27" s="91">
-        <f>F25-F26</f>
+      <c r="F28" s="102">
+        <f>(F25+F26)-F27</f>
         <v>-4706.3984999060631</v>
       </c>
-      <c r="G27" s="92"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="94" t="s">
+      <c r="G28" s="65">
+        <f>(G25+G26)-G27</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="103"/>
+      <c r="I28" s="66" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Renombre los objetos, para poder tener identificado el orden en que deben ser corridos
</commit_message>
<xml_diff>
--- a/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
+++ b/Reportes Ejemplo/Ejemplo_Caratula_SEP_CXP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>concepto</t>
   </si>
@@ -836,7 +836,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1028,9 +1028,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1358,43 +1355,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D15" activeCellId="1" sqref="C1:C1048576 D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="68" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -1402,26 +1397,23 @@
         <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="F2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="70"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="69"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>28</v>
       </c>
@@ -1429,26 +1421,23 @@
         <v>8867057.4600000009</v>
       </c>
       <c r="C3" s="23">
+        <v>164664345.28</v>
+      </c>
+      <c r="D3" s="23">
         <v>27863597.690000001</v>
       </c>
-      <c r="D3" s="23">
-        <v>164664345.28</v>
-      </c>
-      <c r="E3" s="23">
-        <v>27863597.690000001</v>
-      </c>
-      <c r="F3" s="39">
+      <c r="E3" s="39">
         <v>192527942.97</v>
       </c>
-      <c r="G3" s="41">
+      <c r="F3" s="41">
         <v>192527942.97</v>
       </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>29</v>
       </c>
@@ -1456,26 +1445,24 @@
         <v>8866283.2861000001</v>
       </c>
       <c r="C4" s="53">
+        <v>164664345.28</v>
+      </c>
+      <c r="D4" s="53">
         <v>27858891.291499998</v>
       </c>
-      <c r="D4" s="53">
-        <v>164664345.28</v>
-      </c>
-      <c r="E4" s="53">
-        <v>27858891.291499998</v>
-      </c>
-      <c r="F4" s="54">
+      <c r="E4" s="54">
         <v>192523236.5715</v>
       </c>
-      <c r="G4" s="55">
+      <c r="F4" s="55">
         <v>192527942.97</v>
       </c>
-      <c r="H4" s="11">
+      <c r="G4" s="11">
+        <f>E4-F4</f>
         <v>-4706.39849999547</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>34</v>
       </c>
@@ -1489,23 +1476,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="58">
-        <f>C5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="58">
-        <f>D5+E5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="59">
-        <v>0</v>
-      </c>
-      <c r="H5" s="43">
-        <f>G5-F5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>C5+D5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="59">
+        <v>0</v>
+      </c>
+      <c r="G5" s="43">
+        <f>F5-E5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
         <v>4</v>
       </c>
@@ -1513,29 +1496,25 @@
         <v>-0.11949999999999997</v>
       </c>
       <c r="C6" s="56">
+        <v>-2.25</v>
+      </c>
+      <c r="D6" s="58">
         <v>-0.01</v>
       </c>
-      <c r="D6" s="56">
-        <v>-2.25</v>
-      </c>
-      <c r="E6" s="58">
-        <f t="shared" ref="E6:E35" si="0">C6</f>
-        <v>-0.01</v>
-      </c>
-      <c r="F6" s="56">
-        <f t="shared" ref="F6:F35" si="1">D6+E6</f>
+      <c r="E6" s="56">
+        <f t="shared" ref="E6:E34" si="0">C6+D6</f>
         <v>-2.2599999999999998</v>
       </c>
-      <c r="G6" s="61">
+      <c r="F6" s="61">
         <v>2.46</v>
       </c>
-      <c r="H6" s="44">
-        <f t="shared" ref="H6:H36" si="2">G6-F6</f>
+      <c r="G6" s="44">
+        <f t="shared" ref="G6:G34" si="1">F6-E6</f>
         <v>4.72</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49" t="s">
         <v>44</v>
       </c>
@@ -1545,27 +1524,23 @@
       <c r="C7" s="56">
         <v>0</v>
       </c>
-      <c r="D7" s="56">
-        <v>0</v>
-      </c>
-      <c r="E7" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="61">
-        <v>0</v>
-      </c>
-      <c r="H7" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="58">
+        <v>0</v>
+      </c>
+      <c r="E7" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="61">
+        <v>0</v>
+      </c>
+      <c r="G7" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
         <v>5</v>
       </c>
@@ -1573,29 +1548,25 @@
         <v>-1595235.69</v>
       </c>
       <c r="C8" s="56">
+        <v>-29956868.649999999</v>
+      </c>
+      <c r="D8" s="58">
         <v>-119347.66</v>
       </c>
-      <c r="D8" s="56">
-        <v>-29956868.649999999</v>
-      </c>
-      <c r="E8" s="58">
-        <f t="shared" si="0"/>
-        <v>-119347.66</v>
-      </c>
-      <c r="F8" s="56">
-        <f t="shared" si="1"/>
+      <c r="E8" s="56">
+        <f t="shared" si="0"/>
         <v>-30076216.309999999</v>
       </c>
-      <c r="G8" s="61">
+      <c r="F8" s="61">
         <v>-30076216.32</v>
       </c>
-      <c r="H8" s="44">
-        <f t="shared" si="2"/>
+      <c r="G8" s="44">
+        <f t="shared" si="1"/>
         <v>-1.0000001639127731E-2</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
         <v>6</v>
       </c>
@@ -1603,29 +1574,25 @@
         <v>-2.4199999978009146E-2</v>
       </c>
       <c r="C9" s="56">
-        <v>0</v>
-      </c>
-      <c r="D9" s="56">
         <v>-183027.71</v>
       </c>
-      <c r="E9" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="56">
-        <f t="shared" si="1"/>
+      <c r="D9" s="58">
+        <v>0</v>
+      </c>
+      <c r="E9" s="56">
+        <f t="shared" si="0"/>
         <v>-183027.71</v>
       </c>
-      <c r="G9" s="61">
+      <c r="F9" s="61">
         <v>-189332.93</v>
       </c>
-      <c r="H9" s="44">
-        <f t="shared" si="2"/>
+      <c r="G9" s="44">
+        <f t="shared" si="1"/>
         <v>-6305.2200000000012</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
         <v>7</v>
       </c>
@@ -1633,29 +1600,25 @@
         <v>7534.1304000000009</v>
       </c>
       <c r="C10" s="56">
-        <v>0</v>
-      </c>
-      <c r="D10" s="56">
         <v>146948.69</v>
       </c>
-      <c r="E10" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="56">
-        <f t="shared" si="1"/>
+      <c r="D10" s="58">
+        <v>0</v>
+      </c>
+      <c r="E10" s="56">
+        <f t="shared" si="0"/>
         <v>146948.69</v>
       </c>
-      <c r="G10" s="61">
+      <c r="F10" s="61">
         <v>146948.69</v>
       </c>
-      <c r="H10" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
         <v>8</v>
       </c>
@@ -1665,27 +1628,23 @@
       <c r="C11" s="56">
         <v>0</v>
       </c>
-      <c r="D11" s="56">
-        <v>0</v>
-      </c>
-      <c r="E11" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="61">
-        <v>0</v>
-      </c>
-      <c r="H11" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="58">
+        <v>0</v>
+      </c>
+      <c r="E11" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="61">
+        <v>0</v>
+      </c>
+      <c r="G11" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="49" t="s">
         <v>38</v>
       </c>
@@ -1695,27 +1654,23 @@
       <c r="C12" s="56">
         <v>0</v>
       </c>
-      <c r="D12" s="56">
-        <v>0</v>
-      </c>
-      <c r="E12" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="61">
-        <v>0</v>
-      </c>
-      <c r="H12" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="58">
+        <v>0</v>
+      </c>
+      <c r="E12" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="61">
+        <v>0</v>
+      </c>
+      <c r="G12" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="49" t="s">
         <v>35</v>
       </c>
@@ -1725,27 +1680,23 @@
       <c r="C13" s="56">
         <v>0</v>
       </c>
-      <c r="D13" s="56">
-        <v>0</v>
-      </c>
-      <c r="E13" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="61">
-        <v>0</v>
-      </c>
-      <c r="H13" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="58">
+        <v>0</v>
+      </c>
+      <c r="E13" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="61">
+        <v>0</v>
+      </c>
+      <c r="G13" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49" t="s">
         <v>36</v>
       </c>
@@ -1755,27 +1706,23 @@
       <c r="C14" s="56">
         <v>0</v>
       </c>
-      <c r="D14" s="56">
-        <v>0</v>
-      </c>
-      <c r="E14" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="61">
-        <v>0</v>
-      </c>
-      <c r="H14" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="58">
+        <v>0</v>
+      </c>
+      <c r="E14" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="61">
+        <v>0</v>
+      </c>
+      <c r="G14" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49" t="s">
         <v>37</v>
       </c>
@@ -1785,57 +1732,49 @@
       <c r="C15" s="56">
         <v>0</v>
       </c>
-      <c r="D15" s="56">
-        <v>0</v>
-      </c>
-      <c r="E15" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="61">
-        <v>0</v>
-      </c>
-      <c r="H15" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="58">
+        <v>0</v>
+      </c>
+      <c r="E15" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="61">
+        <v>0</v>
+      </c>
+      <c r="G15" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="60">
         <v>-43798.515700000004</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="56">
+        <v>-851206.86</v>
+      </c>
+      <c r="D16" s="58">
         <v>-3502</v>
       </c>
-      <c r="D16" s="56">
-        <v>-851206.86</v>
-      </c>
-      <c r="E16" s="58">
-        <f t="shared" si="0"/>
-        <v>-3502</v>
-      </c>
-      <c r="F16" s="56">
-        <f t="shared" si="1"/>
+      <c r="E16" s="56">
+        <f t="shared" si="0"/>
         <v>-854708.86</v>
       </c>
-      <c r="G16" s="61">
+      <c r="F16" s="61">
         <v>-715496.49</v>
       </c>
-      <c r="H16" s="44">
-        <f t="shared" si="2"/>
+      <c r="G16" s="44">
+        <f t="shared" si="1"/>
         <v>139212.37</v>
       </c>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49" t="s">
         <v>39</v>
       </c>
@@ -1845,27 +1784,23 @@
       <c r="C17" s="56">
         <v>0</v>
       </c>
-      <c r="D17" s="56">
-        <v>0</v>
-      </c>
-      <c r="E17" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="61">
-        <v>0</v>
-      </c>
-      <c r="H17" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="58">
+        <v>0</v>
+      </c>
+      <c r="E17" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="61">
+        <v>0</v>
+      </c>
+      <c r="G17" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49" t="s">
         <v>10</v>
       </c>
@@ -1873,29 +1808,25 @@
         <v>-2336.2399999999998</v>
       </c>
       <c r="C18" s="56">
-        <v>0</v>
-      </c>
-      <c r="D18" s="56">
         <v>-44064.06</v>
       </c>
-      <c r="E18" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="56">
-        <f t="shared" si="1"/>
+      <c r="D18" s="58">
+        <v>0</v>
+      </c>
+      <c r="E18" s="56">
+        <f t="shared" si="0"/>
         <v>-44064.06</v>
       </c>
-      <c r="G18" s="61">
+      <c r="F18" s="61">
         <v>-44064.06</v>
       </c>
-      <c r="H18" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49" t="s">
         <v>40</v>
       </c>
@@ -1905,27 +1836,23 @@
       <c r="C19" s="56">
         <v>0</v>
       </c>
-      <c r="D19" s="56">
-        <v>0</v>
-      </c>
-      <c r="E19" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="61">
-        <v>0</v>
-      </c>
-      <c r="H19" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="58">
+        <v>0</v>
+      </c>
+      <c r="E19" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="61">
+        <v>0</v>
+      </c>
+      <c r="G19" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49" t="s">
         <v>11</v>
       </c>
@@ -1933,29 +1860,25 @@
         <v>-10301.460000000001</v>
       </c>
       <c r="C20" s="56">
+        <v>-204300.61</v>
+      </c>
+      <c r="D20" s="58">
         <v>-23222</v>
       </c>
-      <c r="D20" s="56">
-        <v>-204300.61</v>
-      </c>
-      <c r="E20" s="58">
-        <f t="shared" si="0"/>
-        <v>-23222</v>
-      </c>
-      <c r="F20" s="56">
-        <f t="shared" si="1"/>
+      <c r="E20" s="56">
+        <f t="shared" si="0"/>
         <v>-227522.61</v>
       </c>
-      <c r="G20" s="61">
+      <c r="F20" s="61">
         <v>-227522.62</v>
       </c>
-      <c r="H20" s="44">
-        <f t="shared" si="2"/>
+      <c r="G20" s="44">
+        <f t="shared" si="1"/>
         <v>-1.0000000009313226E-2</v>
       </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49" t="s">
         <v>41</v>
       </c>
@@ -1965,27 +1888,23 @@
       <c r="C21" s="56">
         <v>0</v>
       </c>
-      <c r="D21" s="56">
-        <v>0</v>
-      </c>
-      <c r="E21" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="61">
-        <v>0</v>
-      </c>
-      <c r="H21" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="58">
+        <v>0</v>
+      </c>
+      <c r="E21" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="61">
+        <v>0</v>
+      </c>
+      <c r="G21" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="49" t="s">
         <v>12</v>
       </c>
@@ -1993,29 +1912,25 @@
         <v>2273843.7274000007</v>
       </c>
       <c r="C22" s="56">
+        <v>43785416.359999999</v>
+      </c>
+      <c r="D22" s="58">
         <v>2093582.89</v>
       </c>
-      <c r="D22" s="56">
-        <v>43785416.359999999</v>
-      </c>
-      <c r="E22" s="58">
-        <f t="shared" si="0"/>
-        <v>2093582.89</v>
-      </c>
-      <c r="F22" s="56">
-        <f t="shared" si="1"/>
+      <c r="E22" s="56">
+        <f t="shared" si="0"/>
         <v>45878999.25</v>
       </c>
-      <c r="G22" s="61">
+      <c r="F22" s="61">
         <v>45878999.32</v>
       </c>
-      <c r="H22" s="44">
-        <f t="shared" si="2"/>
+      <c r="G22" s="44">
+        <f t="shared" si="1"/>
         <v>7.0000000298023224E-2</v>
       </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49" t="s">
         <v>13</v>
       </c>
@@ -2023,29 +1938,25 @@
         <v>4812894.9151000027</v>
       </c>
       <c r="C23" s="56">
-        <v>0</v>
-      </c>
-      <c r="D23" s="56">
         <v>91963867.379999995</v>
       </c>
-      <c r="E23" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="56">
-        <f t="shared" si="1"/>
+      <c r="D23" s="58">
+        <v>0</v>
+      </c>
+      <c r="E23" s="56">
+        <f t="shared" si="0"/>
         <v>91963867.379999995</v>
       </c>
-      <c r="G23" s="61">
+      <c r="F23" s="61">
         <v>91963867.390000001</v>
       </c>
-      <c r="H23" s="44">
-        <f t="shared" si="2"/>
+      <c r="G23" s="44">
+        <f t="shared" si="1"/>
         <v>1.000000536441803E-2</v>
       </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
         <v>14</v>
       </c>
@@ -2053,29 +1964,25 @@
         <v>76408.107199999999</v>
       </c>
       <c r="C24" s="56">
+        <v>1468530.25</v>
+      </c>
+      <c r="D24" s="58">
         <v>953091.4</v>
       </c>
-      <c r="D24" s="56">
-        <v>1468530.25</v>
-      </c>
-      <c r="E24" s="58">
-        <f t="shared" si="0"/>
-        <v>953091.4</v>
-      </c>
-      <c r="F24" s="56">
-        <f t="shared" si="1"/>
+      <c r="E24" s="56">
+        <f t="shared" si="0"/>
         <v>2421621.65</v>
       </c>
-      <c r="G24" s="61">
+      <c r="F24" s="61">
         <v>2421621.65</v>
       </c>
-      <c r="H24" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49" t="s">
         <v>15</v>
       </c>
@@ -2083,29 +1990,25 @@
         <v>15693.570400000001</v>
       </c>
       <c r="C25" s="56">
-        <v>0</v>
-      </c>
-      <c r="D25" s="56">
         <v>303015.25</v>
       </c>
-      <c r="E25" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="56">
-        <f t="shared" si="1"/>
+      <c r="D25" s="58">
+        <v>0</v>
+      </c>
+      <c r="E25" s="56">
+        <f t="shared" si="0"/>
         <v>303015.25</v>
       </c>
-      <c r="G25" s="61">
-        <v>0</v>
-      </c>
-      <c r="H25" s="44">
-        <f t="shared" si="2"/>
+      <c r="F25" s="61">
+        <v>0</v>
+      </c>
+      <c r="G25" s="44">
+        <f t="shared" si="1"/>
         <v>-303015.25</v>
       </c>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>42</v>
       </c>
@@ -2115,27 +2018,23 @@
       <c r="C26" s="56">
         <v>0</v>
       </c>
-      <c r="D26" s="56">
-        <v>0</v>
-      </c>
-      <c r="E26" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="61">
-        <v>0</v>
-      </c>
-      <c r="H26" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="58">
+        <v>0</v>
+      </c>
+      <c r="E26" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="61">
+        <v>0</v>
+      </c>
+      <c r="G26" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="49" t="s">
         <v>16</v>
       </c>
@@ -2143,29 +2042,25 @@
         <v>6543.9660000000003</v>
       </c>
       <c r="C27" s="56">
+        <v>122662.46</v>
+      </c>
+      <c r="D27" s="58">
         <v>2140154.81</v>
       </c>
-      <c r="D27" s="56">
-        <v>122662.46</v>
-      </c>
-      <c r="E27" s="58">
-        <f t="shared" si="0"/>
-        <v>2140154.81</v>
-      </c>
-      <c r="F27" s="56">
-        <f t="shared" si="1"/>
+      <c r="E27" s="56">
+        <f t="shared" si="0"/>
         <v>2262817.27</v>
       </c>
-      <c r="G27" s="61">
+      <c r="F27" s="61">
         <v>2262817.25</v>
       </c>
-      <c r="H27" s="44">
-        <f t="shared" si="2"/>
+      <c r="G27" s="44">
+        <f t="shared" si="1"/>
         <v>-2.0000000018626451E-2</v>
       </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49" t="s">
         <v>17</v>
       </c>
@@ -2173,29 +2068,25 @@
         <v>6003.77</v>
       </c>
       <c r="C28" s="56">
+        <v>113052.64</v>
+      </c>
+      <c r="D28" s="58">
         <v>467240.33</v>
       </c>
-      <c r="D28" s="56">
-        <v>113052.64</v>
-      </c>
-      <c r="E28" s="58">
-        <f t="shared" si="0"/>
-        <v>467240.33</v>
-      </c>
-      <c r="F28" s="56">
-        <f t="shared" si="1"/>
+      <c r="E28" s="56">
+        <f t="shared" si="0"/>
         <v>580292.97</v>
       </c>
-      <c r="G28" s="61">
+      <c r="F28" s="61">
         <v>580292.94999999995</v>
       </c>
-      <c r="H28" s="44">
-        <f t="shared" si="2"/>
+      <c r="G28" s="44">
+        <f t="shared" si="1"/>
         <v>-2.0000000018626451E-2</v>
       </c>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49" t="s">
         <v>18</v>
       </c>
@@ -2203,29 +2094,25 @@
         <v>0</v>
       </c>
       <c r="C29" s="56">
+        <v>0</v>
+      </c>
+      <c r="D29" s="58">
         <v>2282441.5299999998</v>
       </c>
-      <c r="D29" s="56">
-        <v>0</v>
-      </c>
-      <c r="E29" s="58">
+      <c r="E29" s="56">
         <f t="shared" si="0"/>
         <v>2282441.5299999998</v>
       </c>
-      <c r="F29" s="56">
-        <f t="shared" si="1"/>
-        <v>2282441.5299999998</v>
-      </c>
-      <c r="G29" s="61">
+      <c r="F29" s="61">
         <v>2282441.52</v>
       </c>
-      <c r="H29" s="44">
-        <f t="shared" si="2"/>
+      <c r="G29" s="44">
+        <f t="shared" si="1"/>
         <v>-9.9999997764825821E-3</v>
       </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="49" t="s">
         <v>19</v>
       </c>
@@ -2233,29 +2120,25 @@
         <v>91197.16</v>
       </c>
       <c r="C30" s="56">
+        <v>1744491.87</v>
+      </c>
+      <c r="D30" s="58">
         <v>28497266.539999999</v>
       </c>
-      <c r="D30" s="56">
-        <v>1744491.87</v>
-      </c>
-      <c r="E30" s="58">
-        <f t="shared" si="0"/>
-        <v>28497266.539999999</v>
-      </c>
-      <c r="F30" s="56">
-        <f t="shared" si="1"/>
+      <c r="E30" s="56">
+        <f t="shared" si="0"/>
         <v>30241758.41</v>
       </c>
-      <c r="G30" s="61">
+      <c r="F30" s="61">
         <v>30074302.809999999</v>
       </c>
-      <c r="H30" s="44">
-        <f t="shared" si="2"/>
+      <c r="G30" s="44">
+        <f t="shared" si="1"/>
         <v>-167455.60000000149</v>
       </c>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
         <v>20</v>
       </c>
@@ -2263,29 +2146,25 @@
         <v>-4699382.6977000032</v>
       </c>
       <c r="C31" s="56">
+        <v>-87473455.150000006</v>
+      </c>
+      <c r="D31" s="58">
         <v>-31340477.59</v>
       </c>
-      <c r="D31" s="56">
-        <v>-87473455.150000006</v>
-      </c>
-      <c r="E31" s="58">
-        <f t="shared" si="0"/>
-        <v>-31340477.59</v>
-      </c>
-      <c r="F31" s="56">
-        <f t="shared" si="1"/>
+      <c r="E31" s="56">
+        <f t="shared" si="0"/>
         <v>-118813932.74000001</v>
       </c>
-      <c r="G31" s="61">
+      <c r="F31" s="61">
         <v>-118656140.56</v>
       </c>
-      <c r="H31" s="44">
-        <f t="shared" si="2"/>
+      <c r="G31" s="44">
+        <f t="shared" si="1"/>
         <v>157792.18000000715</v>
       </c>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="49" t="s">
         <v>43</v>
       </c>
@@ -2295,27 +2174,23 @@
       <c r="C32" s="56">
         <v>0</v>
       </c>
-      <c r="D32" s="56">
-        <v>0</v>
-      </c>
-      <c r="E32" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="61">
-        <v>0</v>
-      </c>
-      <c r="H32" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="58">
+        <v>0</v>
+      </c>
+      <c r="E32" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="61">
+        <v>0</v>
+      </c>
+      <c r="G32" s="44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49" t="s">
         <v>21</v>
       </c>
@@ -2323,29 +2198,25 @@
         <v>0</v>
       </c>
       <c r="C33" s="56">
-        <v>0</v>
-      </c>
-      <c r="D33" s="56">
         <v>6961029.46</v>
       </c>
-      <c r="E33" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="56">
-        <f t="shared" si="1"/>
+      <c r="D33" s="58">
+        <v>0</v>
+      </c>
+      <c r="E33" s="56">
+        <f t="shared" si="0"/>
         <v>6961029.46</v>
       </c>
-      <c r="G33" s="61">
+      <c r="F33" s="61">
         <v>6961029.4400000004</v>
       </c>
-      <c r="H33" s="44">
-        <f t="shared" si="2"/>
+      <c r="G33" s="44">
+        <f t="shared" si="1"/>
         <v>-1.9999999552965164E-2</v>
       </c>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="51" t="s">
         <v>3</v>
       </c>
@@ -2353,29 +2224,25 @@
         <v>0</v>
       </c>
       <c r="C34" s="63">
-        <v>0</v>
-      </c>
-      <c r="D34" s="63">
         <v>-72995.22</v>
       </c>
-      <c r="E34" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="63">
-        <f t="shared" si="1"/>
+      <c r="D34" s="58">
+        <v>0</v>
+      </c>
+      <c r="E34" s="63">
+        <f t="shared" si="0"/>
         <v>-72995.22</v>
       </c>
-      <c r="G34" s="64">
+      <c r="F34" s="64">
         <v>-72995.210000000006</v>
       </c>
-      <c r="H34" s="45">
-        <f t="shared" si="2"/>
+      <c r="G34" s="45">
+        <f t="shared" si="1"/>
         <v>9.9999999947613105E-3</v>
       </c>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="34" t="s">
         <v>30</v>
       </c>
@@ -2384,32 +2251,27 @@
         <v>939064.59939999972</v>
       </c>
       <c r="C35" s="27">
-        <f t="shared" ref="C35:G35" si="3">SUM(C5:C34)</f>
+        <f t="shared" ref="C35:F35" si="2">SUM(C5:C34)</f>
+        <v>27823093.849999987</v>
+      </c>
+      <c r="D35" s="27">
         <v>4947228.2399999984</v>
       </c>
-      <c r="D35" s="27">
-        <f t="shared" si="3"/>
-        <v>27823093.849999987</v>
-      </c>
       <c r="E35" s="27">
-        <f t="shared" si="3"/>
-        <v>4947228.2399999984</v>
+        <f t="shared" si="2"/>
+        <v>32770322.089999996</v>
       </c>
       <c r="F35" s="27">
-        <f t="shared" si="3"/>
-        <v>32770322.089999996</v>
+        <f t="shared" si="2"/>
+        <v>32590555.290000003</v>
       </c>
       <c r="G35" s="27">
-        <f t="shared" si="3"/>
-        <v>32590555.290000003</v>
-      </c>
-      <c r="H35" s="27">
-        <f>SUM(H5:H34)</f>
+        <f>SUM(G5:G34)</f>
         <v>-179766.79999998969</v>
       </c>
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>31</v>
       </c>
@@ -2418,111 +2280,99 @@
         <v>9805347.8854999989</v>
       </c>
       <c r="C36" s="28">
-        <f t="shared" ref="C36:H36" si="4">C4+C35</f>
+        <f t="shared" ref="C36:G36" si="3">C4+C35</f>
+        <v>192487439.13</v>
+      </c>
+      <c r="D36" s="28">
+        <f t="shared" si="3"/>
         <v>32806119.531499997</v>
       </c>
-      <c r="D36" s="28">
-        <f t="shared" si="4"/>
-        <v>192487439.13</v>
-      </c>
       <c r="E36" s="28">
-        <f t="shared" si="4"/>
-        <v>32806119.531499997</v>
+        <f t="shared" si="3"/>
+        <v>225293558.66150001</v>
       </c>
       <c r="F36" s="28">
-        <f t="shared" si="4"/>
-        <v>225293558.66150001</v>
+        <f t="shared" si="3"/>
+        <v>225118498.25999999</v>
       </c>
       <c r="G36" s="28">
-        <f t="shared" si="4"/>
-        <v>225118498.25999999</v>
-      </c>
-      <c r="H36" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-184473.19849998516</v>
       </c>
-      <c r="I36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="29"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="22">
+      <c r="C37" s="16"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="22">
         <v>161333.24</v>
       </c>
-      <c r="H37" s="20"/>
-      <c r="I37" s="17"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="20"/>
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="37" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="30">
         <v>9805347.0899999999</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="14">
+        <v>192473715.09999999</v>
+      </c>
+      <c r="D38" s="14">
         <v>32806116.379999999</v>
       </c>
-      <c r="D38" s="14">
-        <v>192473715.09999999</v>
-      </c>
-      <c r="E38" s="14">
-        <v>32806116.379999999</v>
+      <c r="E38" s="21">
+        <v>225279831.47999999</v>
       </c>
       <c r="F38" s="21">
-        <v>225279831.47999999</v>
-      </c>
-      <c r="G38" s="21">
         <v>225279831.5</v>
       </c>
-      <c r="H38" s="25">
+      <c r="G38" s="25">
         <v>-2.000001072883606E-2</v>
       </c>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H38" s="15"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="4">
-        <f t="shared" ref="B39:F39" si="5">B36+B37-B38</f>
+        <f t="shared" ref="B39:E39" si="4">B36+B37-B38</f>
         <v>0.79549999907612801</v>
       </c>
       <c r="C39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
+        <v>13724.030000001192</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="4"/>
         <v>3.1514999978244305</v>
       </c>
-      <c r="D39" s="4">
-        <f t="shared" si="5"/>
-        <v>13724.030000001192</v>
-      </c>
       <c r="E39" s="4">
-        <f t="shared" si="5"/>
-        <v>3.1514999978244305</v>
+        <f t="shared" si="4"/>
+        <v>13727.181500017643</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="5"/>
-        <v>13727.181500017643</v>
-      </c>
-      <c r="G39" s="4">
-        <f>G36+G37-G38</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="46"/>
-      <c r="I39" s="2"/>
+        <f>F36+F37-F38</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="46"/>
+      <c r="H39" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A5:I34">
     <sortCondition ref="A5:A34"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>